<commit_message>
Changes on Prd Report to notification, review and docoment On Screen Dafination
</commit_message>
<xml_diff>
--- a/RentSure PRD 5.xlsx
+++ b/RentSure PRD 5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Study\Semester - 7\Software Engineering\FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rentsure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2441149D-58E6-420E-AB49-B3FD7F934A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844D6D4E-5B26-4FEF-97DB-B8C1B04AE4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5445" yWindow="2040" windowWidth="21885" windowHeight="11160" tabRatio="216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRD" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="267">
   <si>
     <t>Product Requirement Document (PRD) - Version: 1.0</t>
   </si>
@@ -1048,39 +1048,8 @@
   </si>
   <si>
     <t>&lt;form&gt;
-&lt;input=tenant&gt;
-&lt;input=rating&gt;
-&lt;textarea=review&gt;
-&lt;button=action&gt;</t>
-  </si>
-  <si>
-    <t>&lt;form&gt;
-&lt;textarea=reply&gt;
-&lt;button=submit&gt;</t>
-  </si>
-  <si>
-    <t>&lt;form&gt;
-&lt;select=property&gt;
-&lt;input=file_upload&gt;
-&lt;button=upload_document&gt;</t>
-  </si>
-  <si>
-    <t>&lt;form&gt;
-&lt;input=file_name&gt;
-&lt;input=date&gt;
-&lt;button=action&gt;</t>
-  </si>
-  <si>
-    <t>&lt;form&gt;
 &lt;button=download&gt;
 &lt;button=delete&gt;</t>
-  </si>
-  <si>
-    <t>&lt;form&gt;
-&lt;input=title&gt;
-&lt;textarea=message&gt;
-&lt;input=date&gt;
-&lt;input=status&gt;</t>
   </si>
   <si>
     <t>&lt;form&gt;
@@ -1100,6 +1069,22 @@
   </si>
   <si>
     <t>Feature: 12</t>
+  </si>
+  <si>
+    <t>&lt;form&gt;
+&lt;input=userId&gt;
+&lt;select= property&gt;&lt;button=Show All&gt;</t>
+  </si>
+  <si>
+    <t>&lt;form&gt;
+&lt;input= userId&gt;&lt;textarea=reply&gt;
+&lt;button=submit&gt;</t>
+  </si>
+  <si>
+    <t>&lt;form&gt;
+&lt;input=userId&gt;&lt;select=property&gt;
+&lt;input=file_upload&gt;
+&lt;button=upload_document&gt;</t>
   </si>
 </sst>
 </file>
@@ -1580,6 +1565,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1589,7 +1577,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1615,15 +1609,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1845,8 +1830,8 @@
   </sheetPr>
   <dimension ref="A1:Y948"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1867,16 +1852,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -1923,15 +1908,15 @@
       <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="39"/>
       <c r="G3" s="40"/>
       <c r="H3" s="42"/>
@@ -1954,15 +1939,15 @@
       <c r="Y3" s="4"/>
     </row>
     <row r="4" spans="1:25" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="55" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="39"/>
       <c r="G4" s="40"/>
       <c r="H4" s="42"/>
@@ -1985,13 +1970,13 @@
       <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="39"/>
       <c r="G5" s="40"/>
       <c r="H5" s="42"/>
@@ -2014,15 +1999,15 @@
       <c r="Y5" s="8"/>
     </row>
     <row r="6" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="49" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="51"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="39"/>
       <c r="G6" s="40"/>
       <c r="H6" s="42"/>
@@ -2045,15 +2030,15 @@
       <c r="Y6" s="8"/>
     </row>
     <row r="7" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="51"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="39"/>
       <c r="G7" s="40"/>
       <c r="H7" s="42"/>
@@ -2076,15 +2061,15 @@
       <c r="Y7" s="8"/>
     </row>
     <row r="8" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
       <c r="H8" s="42"/>
@@ -2107,15 +2092,15 @@
       <c r="Y8" s="8"/>
     </row>
     <row r="9" spans="1:25" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49" t="s">
+      <c r="B9" s="51"/>
+      <c r="C9" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="39"/>
       <c r="G9" s="40"/>
       <c r="H9" s="42"/>
@@ -2235,18 +2220,18 @@
       <c r="Y12" s="22"/>
     </row>
     <row r="13" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="13"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -2389,18 +2374,18 @@
       <c r="Y16" s="7"/>
     </row>
     <row r="17" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46" t="s">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
       <c r="I17" s="21"/>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
@@ -2584,18 +2569,18 @@
       <c r="Y21" s="22"/>
     </row>
     <row r="22" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
       <c r="K22" s="22"/>
@@ -2820,18 +2805,18 @@
       <c r="Y27" s="22"/>
     </row>
     <row r="28" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46" t="s">
+      <c r="A28" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46" t="s">
+      <c r="B28" s="43"/>
+      <c r="C28" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
       <c r="I28" s="21"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
@@ -3056,18 +3041,18 @@
       <c r="Y33" s="22"/>
     </row>
     <row r="34" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46" t="s">
+      <c r="B34" s="43"/>
+      <c r="C34" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
       <c r="I34" s="21"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
@@ -3251,18 +3236,18 @@
       <c r="Y38" s="22"/>
     </row>
     <row r="39" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46" t="s">
+      <c r="B39" s="43"/>
+      <c r="C39" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
       <c r="I39" s="6"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
@@ -3445,18 +3430,18 @@
       <c r="Y43" s="22"/>
     </row>
     <row r="44" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="B44" s="46"/>
-      <c r="C44" s="46" t="s">
+      <c r="B44" s="43"/>
+      <c r="C44" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
       <c r="I44" s="6"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
@@ -3555,18 +3540,18 @@
       <c r="X46" s="7"/>
     </row>
     <row r="47" spans="1:25" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46" t="s">
+      <c r="B47" s="43"/>
+      <c r="C47" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43"/>
       <c r="I47" s="6"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
@@ -3745,18 +3730,18 @@
       <c r="X51" s="7"/>
     </row>
     <row r="52" spans="1:24" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="46" t="s">
+      <c r="A52" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46" t="s">
+      <c r="B52" s="43"/>
+      <c r="C52" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="43"/>
       <c r="I52" s="6"/>
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
@@ -3855,18 +3840,18 @@
       <c r="X54" s="7"/>
     </row>
     <row r="55" spans="1:24" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="46"/>
-      <c r="C55" s="46" t="s">
+      <c r="B55" s="43"/>
+      <c r="C55" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="46"/>
-      <c r="H55" s="46"/>
+      <c r="D55" s="43"/>
+      <c r="E55" s="43"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
       <c r="I55" s="6"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
@@ -4005,18 +3990,18 @@
       <c r="X58" s="7"/>
     </row>
     <row r="59" spans="1:24" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="46" t="s">
-        <v>267</v>
-      </c>
-      <c r="B59" s="46"/>
-      <c r="C59" s="46" t="s">
-        <v>266</v>
-      </c>
-      <c r="D59" s="46"/>
-      <c r="E59" s="46"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="46"/>
-      <c r="H59" s="46"/>
+      <c r="A59" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43" t="s">
+        <v>261</v>
+      </c>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="43"/>
       <c r="I59" s="6"/>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
@@ -4085,7 +4070,7 @@
         <v>158</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>159</v>
@@ -4125,7 +4110,7 @@
         <v>160</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="E62" s="31" t="s">
         <v>161</v>
@@ -4155,18 +4140,18 @@
       <c r="X62" s="7"/>
     </row>
     <row r="63" spans="1:24" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="46" t="s">
-        <v>268</v>
-      </c>
-      <c r="B63" s="46"/>
-      <c r="C63" s="46" t="s">
+      <c r="A63" s="43" t="s">
+        <v>263</v>
+      </c>
+      <c r="B63" s="43"/>
+      <c r="C63" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="43"/>
       <c r="I63" s="6"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
@@ -4195,7 +4180,7 @@
         <v>162</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="E64" s="31" t="s">
         <v>163</v>
@@ -4234,9 +4219,7 @@
       <c r="C65" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="D65" s="31" t="s">
-        <v>261</v>
-      </c>
+      <c r="D65" s="31"/>
       <c r="E65" s="31" t="s">
         <v>166</v>
       </c>
@@ -4275,7 +4258,7 @@
         <v>167</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E66" s="31" t="s">
         <v>168</v>
@@ -4305,18 +4288,18 @@
       <c r="X66" s="7"/>
     </row>
     <row r="67" spans="1:24" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="46" t="s">
+      <c r="A67" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="B67" s="46"/>
-      <c r="C67" s="46" t="s">
+      <c r="B67" s="43"/>
+      <c r="C67" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46"/>
-      <c r="G67" s="46"/>
-      <c r="H67" s="46"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="43"/>
       <c r="I67" s="6"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
@@ -4344,9 +4327,7 @@
       <c r="C68" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="D68" s="31" t="s">
-        <v>263</v>
-      </c>
+      <c r="D68" s="31"/>
       <c r="E68" s="31" t="s">
         <v>208</v>
       </c>
@@ -4385,7 +4366,7 @@
         <v>210</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="E69" s="31" t="s">
         <v>211</v>
@@ -4425,7 +4406,7 @@
         <v>212</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E70" s="31" t="s">
         <v>213</v>
@@ -4743,23 +4724,23 @@
     <row r="82" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="44"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="43"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="45"/>
-      <c r="I82" s="43"/>
-      <c r="J82" s="44"/>
-      <c r="K82" s="44"/>
-      <c r="L82" s="45"/>
-      <c r="M82" s="43"/>
-      <c r="N82" s="44"/>
-      <c r="O82" s="45"/>
-      <c r="P82" s="43"/>
-      <c r="Q82" s="44"/>
-      <c r="R82" s="44"/>
-      <c r="S82" s="45"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="46"/>
+      <c r="I82" s="44"/>
+      <c r="J82" s="45"/>
+      <c r="K82" s="45"/>
+      <c r="L82" s="46"/>
+      <c r="M82" s="44"/>
+      <c r="N82" s="45"/>
+      <c r="O82" s="46"/>
+      <c r="P82" s="44"/>
+      <c r="Q82" s="45"/>
+      <c r="R82" s="45"/>
+      <c r="S82" s="46"/>
       <c r="T82" s="7"/>
       <c r="U82" s="7"/>
       <c r="V82" s="7"/>
@@ -4770,23 +4751,23 @@
     <row r="83" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="45"/>
-      <c r="F83" s="43"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="45"/>
-      <c r="I83" s="43"/>
-      <c r="J83" s="44"/>
-      <c r="K83" s="44"/>
-      <c r="L83" s="45"/>
-      <c r="M83" s="43"/>
-      <c r="N83" s="44"/>
-      <c r="O83" s="45"/>
-      <c r="P83" s="43"/>
-      <c r="Q83" s="44"/>
-      <c r="R83" s="44"/>
-      <c r="S83" s="45"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="46"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="45"/>
+      <c r="H83" s="46"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="45"/>
+      <c r="K83" s="45"/>
+      <c r="L83" s="46"/>
+      <c r="M83" s="44"/>
+      <c r="N83" s="45"/>
+      <c r="O83" s="46"/>
+      <c r="P83" s="44"/>
+      <c r="Q83" s="45"/>
+      <c r="R83" s="45"/>
+      <c r="S83" s="46"/>
       <c r="T83" s="7"/>
       <c r="U83" s="7"/>
       <c r="V83" s="7"/>
@@ -4797,23 +4778,23 @@
     <row r="84" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="44"/>
-      <c r="E84" s="45"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="44"/>
-      <c r="H84" s="45"/>
-      <c r="I84" s="43"/>
-      <c r="J84" s="44"/>
-      <c r="K84" s="44"/>
-      <c r="L84" s="45"/>
-      <c r="M84" s="43"/>
-      <c r="N84" s="44"/>
-      <c r="O84" s="45"/>
-      <c r="P84" s="43"/>
-      <c r="Q84" s="44"/>
-      <c r="R84" s="44"/>
-      <c r="S84" s="45"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="45"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="45"/>
+      <c r="H84" s="46"/>
+      <c r="I84" s="44"/>
+      <c r="J84" s="45"/>
+      <c r="K84" s="45"/>
+      <c r="L84" s="46"/>
+      <c r="M84" s="44"/>
+      <c r="N84" s="45"/>
+      <c r="O84" s="46"/>
+      <c r="P84" s="44"/>
+      <c r="Q84" s="45"/>
+      <c r="R84" s="45"/>
+      <c r="S84" s="46"/>
       <c r="T84" s="7"/>
       <c r="U84" s="7"/>
       <c r="V84" s="7"/>
@@ -4824,23 +4805,23 @@
     <row r="85" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="44"/>
-      <c r="E85" s="45"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="45"/>
-      <c r="I85" s="43"/>
-      <c r="J85" s="44"/>
-      <c r="K85" s="44"/>
-      <c r="L85" s="45"/>
-      <c r="M85" s="43"/>
-      <c r="N85" s="44"/>
-      <c r="O85" s="45"/>
-      <c r="P85" s="43"/>
-      <c r="Q85" s="44"/>
-      <c r="R85" s="44"/>
-      <c r="S85" s="45"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="45"/>
+      <c r="E85" s="46"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="45"/>
+      <c r="H85" s="46"/>
+      <c r="I85" s="44"/>
+      <c r="J85" s="45"/>
+      <c r="K85" s="45"/>
+      <c r="L85" s="46"/>
+      <c r="M85" s="44"/>
+      <c r="N85" s="45"/>
+      <c r="O85" s="46"/>
+      <c r="P85" s="44"/>
+      <c r="Q85" s="45"/>
+      <c r="R85" s="45"/>
+      <c r="S85" s="46"/>
       <c r="T85" s="7"/>
       <c r="U85" s="7"/>
       <c r="V85" s="7"/>
@@ -4851,23 +4832,23 @@
     <row r="86" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
-      <c r="C86" s="43"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="45"/>
-      <c r="F86" s="43"/>
-      <c r="G86" s="44"/>
-      <c r="H86" s="45"/>
-      <c r="I86" s="43"/>
-      <c r="J86" s="44"/>
-      <c r="K86" s="44"/>
-      <c r="L86" s="45"/>
-      <c r="M86" s="43"/>
-      <c r="N86" s="44"/>
-      <c r="O86" s="45"/>
-      <c r="P86" s="43"/>
-      <c r="Q86" s="44"/>
-      <c r="R86" s="44"/>
-      <c r="S86" s="45"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="45"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="45"/>
+      <c r="H86" s="46"/>
+      <c r="I86" s="44"/>
+      <c r="J86" s="45"/>
+      <c r="K86" s="45"/>
+      <c r="L86" s="46"/>
+      <c r="M86" s="44"/>
+      <c r="N86" s="45"/>
+      <c r="O86" s="46"/>
+      <c r="P86" s="44"/>
+      <c r="Q86" s="45"/>
+      <c r="R86" s="45"/>
+      <c r="S86" s="46"/>
       <c r="T86" s="7"/>
       <c r="U86" s="7"/>
       <c r="V86" s="7"/>
@@ -4878,23 +4859,23 @@
     <row r="87" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
-      <c r="C87" s="43"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="45"/>
-      <c r="F87" s="43"/>
-      <c r="G87" s="44"/>
-      <c r="H87" s="45"/>
-      <c r="I87" s="43"/>
-      <c r="J87" s="44"/>
-      <c r="K87" s="44"/>
-      <c r="L87" s="45"/>
-      <c r="M87" s="43"/>
-      <c r="N87" s="44"/>
-      <c r="O87" s="45"/>
-      <c r="P87" s="43"/>
-      <c r="Q87" s="44"/>
-      <c r="R87" s="44"/>
-      <c r="S87" s="45"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="46"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="45"/>
+      <c r="H87" s="46"/>
+      <c r="I87" s="44"/>
+      <c r="J87" s="45"/>
+      <c r="K87" s="45"/>
+      <c r="L87" s="46"/>
+      <c r="M87" s="44"/>
+      <c r="N87" s="45"/>
+      <c r="O87" s="46"/>
+      <c r="P87" s="44"/>
+      <c r="Q87" s="45"/>
+      <c r="R87" s="45"/>
+      <c r="S87" s="46"/>
       <c r="T87" s="7"/>
       <c r="U87" s="7"/>
       <c r="V87" s="7"/>
@@ -4905,23 +4886,23 @@
     <row r="88" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
-      <c r="C88" s="43"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="45"/>
-      <c r="F88" s="43"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="45"/>
-      <c r="I88" s="43"/>
-      <c r="J88" s="44"/>
-      <c r="K88" s="44"/>
-      <c r="L88" s="45"/>
-      <c r="M88" s="43"/>
-      <c r="N88" s="44"/>
-      <c r="O88" s="45"/>
-      <c r="P88" s="43"/>
-      <c r="Q88" s="44"/>
-      <c r="R88" s="44"/>
-      <c r="S88" s="45"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="45"/>
+      <c r="E88" s="46"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="45"/>
+      <c r="H88" s="46"/>
+      <c r="I88" s="44"/>
+      <c r="J88" s="45"/>
+      <c r="K88" s="45"/>
+      <c r="L88" s="46"/>
+      <c r="M88" s="44"/>
+      <c r="N88" s="45"/>
+      <c r="O88" s="46"/>
+      <c r="P88" s="44"/>
+      <c r="Q88" s="45"/>
+      <c r="R88" s="45"/>
+      <c r="S88" s="46"/>
       <c r="T88" s="7"/>
       <c r="U88" s="7"/>
       <c r="V88" s="7"/>
@@ -4932,23 +4913,23 @@
     <row r="89" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
-      <c r="C89" s="43"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="45"/>
-      <c r="F89" s="43"/>
-      <c r="G89" s="44"/>
-      <c r="H89" s="45"/>
-      <c r="I89" s="43"/>
-      <c r="J89" s="44"/>
-      <c r="K89" s="44"/>
-      <c r="L89" s="45"/>
-      <c r="M89" s="43"/>
-      <c r="N89" s="44"/>
-      <c r="O89" s="45"/>
-      <c r="P89" s="43"/>
-      <c r="Q89" s="44"/>
-      <c r="R89" s="44"/>
-      <c r="S89" s="45"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="45"/>
+      <c r="E89" s="46"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="45"/>
+      <c r="H89" s="46"/>
+      <c r="I89" s="44"/>
+      <c r="J89" s="45"/>
+      <c r="K89" s="45"/>
+      <c r="L89" s="46"/>
+      <c r="M89" s="44"/>
+      <c r="N89" s="45"/>
+      <c r="O89" s="46"/>
+      <c r="P89" s="44"/>
+      <c r="Q89" s="45"/>
+      <c r="R89" s="45"/>
+      <c r="S89" s="46"/>
       <c r="T89" s="7"/>
       <c r="U89" s="7"/>
       <c r="V89" s="7"/>
@@ -4959,23 +4940,23 @@
     <row r="90" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
-      <c r="C90" s="43"/>
-      <c r="D90" s="44"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="43"/>
-      <c r="G90" s="44"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="43"/>
-      <c r="J90" s="44"/>
-      <c r="K90" s="44"/>
-      <c r="L90" s="45"/>
-      <c r="M90" s="43"/>
-      <c r="N90" s="44"/>
-      <c r="O90" s="45"/>
-      <c r="P90" s="43"/>
-      <c r="Q90" s="44"/>
-      <c r="R90" s="44"/>
-      <c r="S90" s="45"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="45"/>
+      <c r="E90" s="46"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="45"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="44"/>
+      <c r="J90" s="45"/>
+      <c r="K90" s="45"/>
+      <c r="L90" s="46"/>
+      <c r="M90" s="44"/>
+      <c r="N90" s="45"/>
+      <c r="O90" s="46"/>
+      <c r="P90" s="44"/>
+      <c r="Q90" s="45"/>
+      <c r="R90" s="45"/>
+      <c r="S90" s="46"/>
       <c r="T90" s="7"/>
       <c r="U90" s="7"/>
       <c r="V90" s="7"/>
@@ -4986,23 +4967,23 @@
     <row r="91" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
-      <c r="C91" s="43"/>
-      <c r="D91" s="44"/>
-      <c r="E91" s="45"/>
-      <c r="F91" s="43"/>
-      <c r="G91" s="44"/>
-      <c r="H91" s="45"/>
-      <c r="I91" s="43"/>
-      <c r="J91" s="44"/>
-      <c r="K91" s="44"/>
-      <c r="L91" s="45"/>
-      <c r="M91" s="43"/>
-      <c r="N91" s="44"/>
-      <c r="O91" s="45"/>
-      <c r="P91" s="43"/>
-      <c r="Q91" s="44"/>
-      <c r="R91" s="44"/>
-      <c r="S91" s="45"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="45"/>
+      <c r="E91" s="46"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="45"/>
+      <c r="H91" s="46"/>
+      <c r="I91" s="44"/>
+      <c r="J91" s="45"/>
+      <c r="K91" s="45"/>
+      <c r="L91" s="46"/>
+      <c r="M91" s="44"/>
+      <c r="N91" s="45"/>
+      <c r="O91" s="46"/>
+      <c r="P91" s="44"/>
+      <c r="Q91" s="45"/>
+      <c r="R91" s="45"/>
+      <c r="S91" s="46"/>
       <c r="T91" s="7"/>
       <c r="U91" s="7"/>
       <c r="V91" s="7"/>
@@ -5013,23 +4994,23 @@
     <row r="92" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
-      <c r="C92" s="43"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="45"/>
-      <c r="F92" s="43"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="45"/>
-      <c r="I92" s="43"/>
-      <c r="J92" s="44"/>
-      <c r="K92" s="44"/>
-      <c r="L92" s="45"/>
-      <c r="M92" s="43"/>
-      <c r="N92" s="44"/>
-      <c r="O92" s="45"/>
-      <c r="P92" s="43"/>
-      <c r="Q92" s="44"/>
-      <c r="R92" s="44"/>
-      <c r="S92" s="45"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="45"/>
+      <c r="E92" s="46"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="45"/>
+      <c r="H92" s="46"/>
+      <c r="I92" s="44"/>
+      <c r="J92" s="45"/>
+      <c r="K92" s="45"/>
+      <c r="L92" s="46"/>
+      <c r="M92" s="44"/>
+      <c r="N92" s="45"/>
+      <c r="O92" s="46"/>
+      <c r="P92" s="44"/>
+      <c r="Q92" s="45"/>
+      <c r="R92" s="45"/>
+      <c r="S92" s="46"/>
       <c r="T92" s="7"/>
       <c r="U92" s="7"/>
       <c r="V92" s="7"/>
@@ -5040,23 +5021,23 @@
     <row r="93" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
-      <c r="C93" s="43"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="45"/>
-      <c r="F93" s="43"/>
-      <c r="G93" s="44"/>
-      <c r="H93" s="45"/>
-      <c r="I93" s="43"/>
-      <c r="J93" s="44"/>
-      <c r="K93" s="44"/>
-      <c r="L93" s="45"/>
-      <c r="M93" s="43"/>
-      <c r="N93" s="44"/>
-      <c r="O93" s="45"/>
-      <c r="P93" s="43"/>
-      <c r="Q93" s="44"/>
-      <c r="R93" s="44"/>
-      <c r="S93" s="45"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="45"/>
+      <c r="E93" s="46"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="45"/>
+      <c r="H93" s="46"/>
+      <c r="I93" s="44"/>
+      <c r="J93" s="45"/>
+      <c r="K93" s="45"/>
+      <c r="L93" s="46"/>
+      <c r="M93" s="44"/>
+      <c r="N93" s="45"/>
+      <c r="O93" s="46"/>
+      <c r="P93" s="44"/>
+      <c r="Q93" s="45"/>
+      <c r="R93" s="45"/>
+      <c r="S93" s="46"/>
       <c r="T93" s="7"/>
       <c r="U93" s="7"/>
       <c r="V93" s="7"/>
@@ -5067,23 +5048,23 @@
     <row r="94" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
-      <c r="C94" s="43"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="45"/>
-      <c r="F94" s="43"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="45"/>
-      <c r="I94" s="43"/>
-      <c r="J94" s="44"/>
-      <c r="K94" s="44"/>
-      <c r="L94" s="45"/>
-      <c r="M94" s="43"/>
-      <c r="N94" s="44"/>
-      <c r="O94" s="45"/>
-      <c r="P94" s="43"/>
-      <c r="Q94" s="44"/>
-      <c r="R94" s="44"/>
-      <c r="S94" s="45"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="45"/>
+      <c r="E94" s="46"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="45"/>
+      <c r="H94" s="46"/>
+      <c r="I94" s="44"/>
+      <c r="J94" s="45"/>
+      <c r="K94" s="45"/>
+      <c r="L94" s="46"/>
+      <c r="M94" s="44"/>
+      <c r="N94" s="45"/>
+      <c r="O94" s="46"/>
+      <c r="P94" s="44"/>
+      <c r="Q94" s="45"/>
+      <c r="R94" s="45"/>
+      <c r="S94" s="46"/>
       <c r="T94" s="7"/>
       <c r="U94" s="7"/>
       <c r="V94" s="7"/>
@@ -5094,23 +5075,23 @@
     <row r="95" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
-      <c r="C95" s="43"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="45"/>
-      <c r="F95" s="43"/>
-      <c r="G95" s="44"/>
-      <c r="H95" s="45"/>
-      <c r="I95" s="43"/>
-      <c r="J95" s="44"/>
-      <c r="K95" s="44"/>
-      <c r="L95" s="45"/>
-      <c r="M95" s="43"/>
-      <c r="N95" s="44"/>
-      <c r="O95" s="45"/>
-      <c r="P95" s="43"/>
-      <c r="Q95" s="44"/>
-      <c r="R95" s="44"/>
-      <c r="S95" s="45"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="45"/>
+      <c r="E95" s="46"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="45"/>
+      <c r="H95" s="46"/>
+      <c r="I95" s="44"/>
+      <c r="J95" s="45"/>
+      <c r="K95" s="45"/>
+      <c r="L95" s="46"/>
+      <c r="M95" s="44"/>
+      <c r="N95" s="45"/>
+      <c r="O95" s="46"/>
+      <c r="P95" s="44"/>
+      <c r="Q95" s="45"/>
+      <c r="R95" s="45"/>
+      <c r="S95" s="46"/>
       <c r="T95" s="7"/>
       <c r="U95" s="7"/>
       <c r="V95" s="7"/>
@@ -5121,23 +5102,23 @@
     <row r="96" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
-      <c r="C96" s="43"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="45"/>
-      <c r="F96" s="43"/>
-      <c r="G96" s="44"/>
-      <c r="H96" s="45"/>
-      <c r="I96" s="43"/>
-      <c r="J96" s="44"/>
-      <c r="K96" s="44"/>
-      <c r="L96" s="45"/>
-      <c r="M96" s="43"/>
-      <c r="N96" s="44"/>
-      <c r="O96" s="45"/>
-      <c r="P96" s="43"/>
-      <c r="Q96" s="44"/>
-      <c r="R96" s="44"/>
-      <c r="S96" s="45"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="45"/>
+      <c r="E96" s="46"/>
+      <c r="F96" s="44"/>
+      <c r="G96" s="45"/>
+      <c r="H96" s="46"/>
+      <c r="I96" s="44"/>
+      <c r="J96" s="45"/>
+      <c r="K96" s="45"/>
+      <c r="L96" s="46"/>
+      <c r="M96" s="44"/>
+      <c r="N96" s="45"/>
+      <c r="O96" s="46"/>
+      <c r="P96" s="44"/>
+      <c r="Q96" s="45"/>
+      <c r="R96" s="45"/>
+      <c r="S96" s="46"/>
       <c r="T96" s="7"/>
       <c r="U96" s="7"/>
       <c r="V96" s="7"/>
@@ -5148,23 +5129,23 @@
     <row r="97" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
-      <c r="C97" s="43"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="45"/>
-      <c r="F97" s="43"/>
-      <c r="G97" s="44"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="43"/>
-      <c r="J97" s="44"/>
-      <c r="K97" s="44"/>
-      <c r="L97" s="45"/>
-      <c r="M97" s="43"/>
-      <c r="N97" s="44"/>
-      <c r="O97" s="45"/>
-      <c r="P97" s="43"/>
-      <c r="Q97" s="44"/>
-      <c r="R97" s="44"/>
-      <c r="S97" s="45"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="45"/>
+      <c r="E97" s="46"/>
+      <c r="F97" s="44"/>
+      <c r="G97" s="45"/>
+      <c r="H97" s="46"/>
+      <c r="I97" s="44"/>
+      <c r="J97" s="45"/>
+      <c r="K97" s="45"/>
+      <c r="L97" s="46"/>
+      <c r="M97" s="44"/>
+      <c r="N97" s="45"/>
+      <c r="O97" s="46"/>
+      <c r="P97" s="44"/>
+      <c r="Q97" s="45"/>
+      <c r="R97" s="45"/>
+      <c r="S97" s="46"/>
       <c r="T97" s="7"/>
       <c r="U97" s="7"/>
       <c r="V97" s="7"/>
@@ -5175,23 +5156,23 @@
     <row r="98" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
-      <c r="C98" s="43"/>
-      <c r="D98" s="44"/>
-      <c r="E98" s="45"/>
-      <c r="F98" s="43"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="45"/>
-      <c r="I98" s="43"/>
-      <c r="J98" s="44"/>
-      <c r="K98" s="44"/>
-      <c r="L98" s="45"/>
-      <c r="M98" s="43"/>
-      <c r="N98" s="44"/>
-      <c r="O98" s="45"/>
-      <c r="P98" s="43"/>
-      <c r="Q98" s="44"/>
-      <c r="R98" s="44"/>
-      <c r="S98" s="45"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="45"/>
+      <c r="E98" s="46"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="45"/>
+      <c r="H98" s="46"/>
+      <c r="I98" s="44"/>
+      <c r="J98" s="45"/>
+      <c r="K98" s="45"/>
+      <c r="L98" s="46"/>
+      <c r="M98" s="44"/>
+      <c r="N98" s="45"/>
+      <c r="O98" s="46"/>
+      <c r="P98" s="44"/>
+      <c r="Q98" s="45"/>
+      <c r="R98" s="45"/>
+      <c r="S98" s="46"/>
       <c r="T98" s="7"/>
       <c r="U98" s="7"/>
       <c r="V98" s="7"/>
@@ -5202,23 +5183,23 @@
     <row r="99" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
-      <c r="C99" s="43"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="45"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="44"/>
-      <c r="H99" s="45"/>
-      <c r="I99" s="43"/>
-      <c r="J99" s="44"/>
-      <c r="K99" s="44"/>
-      <c r="L99" s="45"/>
-      <c r="M99" s="43"/>
-      <c r="N99" s="44"/>
-      <c r="O99" s="45"/>
-      <c r="P99" s="43"/>
-      <c r="Q99" s="44"/>
-      <c r="R99" s="44"/>
-      <c r="S99" s="45"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="45"/>
+      <c r="E99" s="46"/>
+      <c r="F99" s="44"/>
+      <c r="G99" s="45"/>
+      <c r="H99" s="46"/>
+      <c r="I99" s="44"/>
+      <c r="J99" s="45"/>
+      <c r="K99" s="45"/>
+      <c r="L99" s="46"/>
+      <c r="M99" s="44"/>
+      <c r="N99" s="45"/>
+      <c r="O99" s="46"/>
+      <c r="P99" s="44"/>
+      <c r="Q99" s="45"/>
+      <c r="R99" s="45"/>
+      <c r="S99" s="46"/>
       <c r="T99" s="7"/>
       <c r="U99" s="7"/>
       <c r="V99" s="7"/>
@@ -5229,23 +5210,23 @@
     <row r="100" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
-      <c r="C100" s="43"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="45"/>
-      <c r="F100" s="43"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="45"/>
-      <c r="I100" s="43"/>
-      <c r="J100" s="44"/>
-      <c r="K100" s="44"/>
-      <c r="L100" s="45"/>
-      <c r="M100" s="43"/>
-      <c r="N100" s="44"/>
-      <c r="O100" s="45"/>
-      <c r="P100" s="43"/>
-      <c r="Q100" s="44"/>
-      <c r="R100" s="44"/>
-      <c r="S100" s="45"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="45"/>
+      <c r="E100" s="46"/>
+      <c r="F100" s="44"/>
+      <c r="G100" s="45"/>
+      <c r="H100" s="46"/>
+      <c r="I100" s="44"/>
+      <c r="J100" s="45"/>
+      <c r="K100" s="45"/>
+      <c r="L100" s="46"/>
+      <c r="M100" s="44"/>
+      <c r="N100" s="45"/>
+      <c r="O100" s="46"/>
+      <c r="P100" s="44"/>
+      <c r="Q100" s="45"/>
+      <c r="R100" s="45"/>
+      <c r="S100" s="46"/>
       <c r="T100" s="7"/>
       <c r="U100" s="7"/>
       <c r="V100" s="7"/>
@@ -5256,23 +5237,23 @@
     <row r="101" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
-      <c r="C101" s="43"/>
-      <c r="D101" s="44"/>
-      <c r="E101" s="45"/>
-      <c r="F101" s="43"/>
-      <c r="G101" s="44"/>
-      <c r="H101" s="45"/>
-      <c r="I101" s="43"/>
-      <c r="J101" s="44"/>
-      <c r="K101" s="44"/>
-      <c r="L101" s="45"/>
-      <c r="M101" s="43"/>
-      <c r="N101" s="44"/>
-      <c r="O101" s="45"/>
-      <c r="P101" s="43"/>
-      <c r="Q101" s="44"/>
-      <c r="R101" s="44"/>
-      <c r="S101" s="45"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="45"/>
+      <c r="E101" s="46"/>
+      <c r="F101" s="44"/>
+      <c r="G101" s="45"/>
+      <c r="H101" s="46"/>
+      <c r="I101" s="44"/>
+      <c r="J101" s="45"/>
+      <c r="K101" s="45"/>
+      <c r="L101" s="46"/>
+      <c r="M101" s="44"/>
+      <c r="N101" s="45"/>
+      <c r="O101" s="46"/>
+      <c r="P101" s="44"/>
+      <c r="Q101" s="45"/>
+      <c r="R101" s="45"/>
+      <c r="S101" s="46"/>
       <c r="T101" s="7"/>
       <c r="U101" s="7"/>
       <c r="V101" s="7"/>
@@ -5283,23 +5264,23 @@
     <row r="102" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
-      <c r="C102" s="43"/>
-      <c r="D102" s="44"/>
-      <c r="E102" s="45"/>
-      <c r="F102" s="43"/>
-      <c r="G102" s="44"/>
-      <c r="H102" s="45"/>
-      <c r="I102" s="43"/>
-      <c r="J102" s="44"/>
-      <c r="K102" s="44"/>
-      <c r="L102" s="45"/>
-      <c r="M102" s="43"/>
-      <c r="N102" s="44"/>
-      <c r="O102" s="45"/>
-      <c r="P102" s="43"/>
-      <c r="Q102" s="44"/>
-      <c r="R102" s="44"/>
-      <c r="S102" s="45"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="45"/>
+      <c r="E102" s="46"/>
+      <c r="F102" s="44"/>
+      <c r="G102" s="45"/>
+      <c r="H102" s="46"/>
+      <c r="I102" s="44"/>
+      <c r="J102" s="45"/>
+      <c r="K102" s="45"/>
+      <c r="L102" s="46"/>
+      <c r="M102" s="44"/>
+      <c r="N102" s="45"/>
+      <c r="O102" s="46"/>
+      <c r="P102" s="44"/>
+      <c r="Q102" s="45"/>
+      <c r="R102" s="45"/>
+      <c r="S102" s="46"/>
       <c r="T102" s="7"/>
       <c r="U102" s="7"/>
       <c r="V102" s="7"/>
@@ -5310,23 +5291,23 @@
     <row r="103" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
-      <c r="C103" s="43"/>
-      <c r="D103" s="44"/>
-      <c r="E103" s="45"/>
-      <c r="F103" s="43"/>
-      <c r="G103" s="44"/>
-      <c r="H103" s="45"/>
-      <c r="I103" s="43"/>
-      <c r="J103" s="44"/>
-      <c r="K103" s="44"/>
-      <c r="L103" s="45"/>
-      <c r="M103" s="43"/>
-      <c r="N103" s="44"/>
-      <c r="O103" s="45"/>
-      <c r="P103" s="43"/>
-      <c r="Q103" s="44"/>
-      <c r="R103" s="44"/>
-      <c r="S103" s="45"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="45"/>
+      <c r="E103" s="46"/>
+      <c r="F103" s="44"/>
+      <c r="G103" s="45"/>
+      <c r="H103" s="46"/>
+      <c r="I103" s="44"/>
+      <c r="J103" s="45"/>
+      <c r="K103" s="45"/>
+      <c r="L103" s="46"/>
+      <c r="M103" s="44"/>
+      <c r="N103" s="45"/>
+      <c r="O103" s="46"/>
+      <c r="P103" s="44"/>
+      <c r="Q103" s="45"/>
+      <c r="R103" s="45"/>
+      <c r="S103" s="46"/>
       <c r="T103" s="7"/>
       <c r="U103" s="7"/>
       <c r="V103" s="7"/>
@@ -5337,23 +5318,23 @@
     <row r="104" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
-      <c r="C104" s="43"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="45"/>
-      <c r="F104" s="43"/>
-      <c r="G104" s="44"/>
-      <c r="H104" s="45"/>
-      <c r="I104" s="43"/>
-      <c r="J104" s="44"/>
-      <c r="K104" s="44"/>
-      <c r="L104" s="45"/>
-      <c r="M104" s="43"/>
-      <c r="N104" s="44"/>
-      <c r="O104" s="45"/>
-      <c r="P104" s="43"/>
-      <c r="Q104" s="44"/>
-      <c r="R104" s="44"/>
-      <c r="S104" s="45"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="45"/>
+      <c r="E104" s="46"/>
+      <c r="F104" s="44"/>
+      <c r="G104" s="45"/>
+      <c r="H104" s="46"/>
+      <c r="I104" s="44"/>
+      <c r="J104" s="45"/>
+      <c r="K104" s="45"/>
+      <c r="L104" s="46"/>
+      <c r="M104" s="44"/>
+      <c r="N104" s="45"/>
+      <c r="O104" s="46"/>
+      <c r="P104" s="44"/>
+      <c r="Q104" s="45"/>
+      <c r="R104" s="45"/>
+      <c r="S104" s="46"/>
       <c r="T104" s="7"/>
       <c r="U104" s="7"/>
       <c r="V104" s="7"/>
@@ -5364,23 +5345,23 @@
     <row r="105" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
-      <c r="C105" s="43"/>
-      <c r="D105" s="44"/>
-      <c r="E105" s="45"/>
-      <c r="F105" s="43"/>
-      <c r="G105" s="44"/>
-      <c r="H105" s="45"/>
-      <c r="I105" s="43"/>
-      <c r="J105" s="44"/>
-      <c r="K105" s="44"/>
-      <c r="L105" s="45"/>
-      <c r="M105" s="43"/>
-      <c r="N105" s="44"/>
-      <c r="O105" s="45"/>
-      <c r="P105" s="43"/>
-      <c r="Q105" s="44"/>
-      <c r="R105" s="44"/>
-      <c r="S105" s="45"/>
+      <c r="C105" s="44"/>
+      <c r="D105" s="45"/>
+      <c r="E105" s="46"/>
+      <c r="F105" s="44"/>
+      <c r="G105" s="45"/>
+      <c r="H105" s="46"/>
+      <c r="I105" s="44"/>
+      <c r="J105" s="45"/>
+      <c r="K105" s="45"/>
+      <c r="L105" s="46"/>
+      <c r="M105" s="44"/>
+      <c r="N105" s="45"/>
+      <c r="O105" s="46"/>
+      <c r="P105" s="44"/>
+      <c r="Q105" s="45"/>
+      <c r="R105" s="45"/>
+      <c r="S105" s="46"/>
       <c r="T105" s="7"/>
       <c r="U105" s="7"/>
       <c r="V105" s="7"/>
@@ -5391,23 +5372,23 @@
     <row r="106" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
-      <c r="C106" s="43"/>
-      <c r="D106" s="44"/>
-      <c r="E106" s="45"/>
-      <c r="F106" s="43"/>
-      <c r="G106" s="44"/>
-      <c r="H106" s="45"/>
-      <c r="I106" s="43"/>
-      <c r="J106" s="44"/>
-      <c r="K106" s="44"/>
-      <c r="L106" s="45"/>
-      <c r="M106" s="43"/>
-      <c r="N106" s="44"/>
-      <c r="O106" s="45"/>
-      <c r="P106" s="43"/>
-      <c r="Q106" s="44"/>
-      <c r="R106" s="44"/>
-      <c r="S106" s="45"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="45"/>
+      <c r="E106" s="46"/>
+      <c r="F106" s="44"/>
+      <c r="G106" s="45"/>
+      <c r="H106" s="46"/>
+      <c r="I106" s="44"/>
+      <c r="J106" s="45"/>
+      <c r="K106" s="45"/>
+      <c r="L106" s="46"/>
+      <c r="M106" s="44"/>
+      <c r="N106" s="45"/>
+      <c r="O106" s="46"/>
+      <c r="P106" s="44"/>
+      <c r="Q106" s="45"/>
+      <c r="R106" s="45"/>
+      <c r="S106" s="46"/>
       <c r="T106" s="7"/>
       <c r="U106" s="7"/>
       <c r="V106" s="7"/>
@@ -5418,23 +5399,23 @@
     <row r="107" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
-      <c r="C107" s="43"/>
-      <c r="D107" s="44"/>
-      <c r="E107" s="45"/>
-      <c r="F107" s="43"/>
-      <c r="G107" s="44"/>
-      <c r="H107" s="45"/>
-      <c r="I107" s="43"/>
-      <c r="J107" s="44"/>
-      <c r="K107" s="44"/>
-      <c r="L107" s="45"/>
-      <c r="M107" s="43"/>
-      <c r="N107" s="44"/>
-      <c r="O107" s="45"/>
-      <c r="P107" s="43"/>
-      <c r="Q107" s="44"/>
-      <c r="R107" s="44"/>
-      <c r="S107" s="45"/>
+      <c r="C107" s="44"/>
+      <c r="D107" s="45"/>
+      <c r="E107" s="46"/>
+      <c r="F107" s="44"/>
+      <c r="G107" s="45"/>
+      <c r="H107" s="46"/>
+      <c r="I107" s="44"/>
+      <c r="J107" s="45"/>
+      <c r="K107" s="45"/>
+      <c r="L107" s="46"/>
+      <c r="M107" s="44"/>
+      <c r="N107" s="45"/>
+      <c r="O107" s="46"/>
+      <c r="P107" s="44"/>
+      <c r="Q107" s="45"/>
+      <c r="R107" s="45"/>
+      <c r="S107" s="46"/>
       <c r="T107" s="7"/>
       <c r="U107" s="7"/>
       <c r="V107" s="7"/>
@@ -5445,23 +5426,23 @@
     <row r="108" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
-      <c r="C108" s="43"/>
-      <c r="D108" s="44"/>
-      <c r="E108" s="45"/>
-      <c r="F108" s="43"/>
-      <c r="G108" s="44"/>
-      <c r="H108" s="45"/>
-      <c r="I108" s="43"/>
-      <c r="J108" s="44"/>
-      <c r="K108" s="44"/>
-      <c r="L108" s="45"/>
-      <c r="M108" s="43"/>
-      <c r="N108" s="44"/>
-      <c r="O108" s="45"/>
-      <c r="P108" s="43"/>
-      <c r="Q108" s="44"/>
-      <c r="R108" s="44"/>
-      <c r="S108" s="45"/>
+      <c r="C108" s="44"/>
+      <c r="D108" s="45"/>
+      <c r="E108" s="46"/>
+      <c r="F108" s="44"/>
+      <c r="G108" s="45"/>
+      <c r="H108" s="46"/>
+      <c r="I108" s="44"/>
+      <c r="J108" s="45"/>
+      <c r="K108" s="45"/>
+      <c r="L108" s="46"/>
+      <c r="M108" s="44"/>
+      <c r="N108" s="45"/>
+      <c r="O108" s="46"/>
+      <c r="P108" s="44"/>
+      <c r="Q108" s="45"/>
+      <c r="R108" s="45"/>
+      <c r="S108" s="46"/>
       <c r="T108" s="7"/>
       <c r="U108" s="7"/>
       <c r="V108" s="7"/>
@@ -5472,23 +5453,23 @@
     <row r="109" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
-      <c r="C109" s="43"/>
-      <c r="D109" s="44"/>
-      <c r="E109" s="45"/>
-      <c r="F109" s="43"/>
-      <c r="G109" s="44"/>
-      <c r="H109" s="45"/>
-      <c r="I109" s="43"/>
-      <c r="J109" s="44"/>
-      <c r="K109" s="44"/>
-      <c r="L109" s="45"/>
-      <c r="M109" s="43"/>
-      <c r="N109" s="44"/>
-      <c r="O109" s="45"/>
-      <c r="P109" s="43"/>
-      <c r="Q109" s="44"/>
-      <c r="R109" s="44"/>
-      <c r="S109" s="45"/>
+      <c r="C109" s="44"/>
+      <c r="D109" s="45"/>
+      <c r="E109" s="46"/>
+      <c r="F109" s="44"/>
+      <c r="G109" s="45"/>
+      <c r="H109" s="46"/>
+      <c r="I109" s="44"/>
+      <c r="J109" s="45"/>
+      <c r="K109" s="45"/>
+      <c r="L109" s="46"/>
+      <c r="M109" s="44"/>
+      <c r="N109" s="45"/>
+      <c r="O109" s="46"/>
+      <c r="P109" s="44"/>
+      <c r="Q109" s="45"/>
+      <c r="R109" s="45"/>
+      <c r="S109" s="46"/>
       <c r="T109" s="7"/>
       <c r="U109" s="7"/>
       <c r="V109" s="7"/>
@@ -5499,23 +5480,23 @@
     <row r="110" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
-      <c r="C110" s="43"/>
-      <c r="D110" s="44"/>
-      <c r="E110" s="45"/>
-      <c r="F110" s="43"/>
-      <c r="G110" s="44"/>
-      <c r="H110" s="45"/>
-      <c r="I110" s="43"/>
-      <c r="J110" s="44"/>
-      <c r="K110" s="44"/>
-      <c r="L110" s="45"/>
-      <c r="M110" s="43"/>
-      <c r="N110" s="44"/>
-      <c r="O110" s="45"/>
-      <c r="P110" s="43"/>
-      <c r="Q110" s="44"/>
-      <c r="R110" s="44"/>
-      <c r="S110" s="45"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="45"/>
+      <c r="E110" s="46"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="45"/>
+      <c r="H110" s="46"/>
+      <c r="I110" s="44"/>
+      <c r="J110" s="45"/>
+      <c r="K110" s="45"/>
+      <c r="L110" s="46"/>
+      <c r="M110" s="44"/>
+      <c r="N110" s="45"/>
+      <c r="O110" s="46"/>
+      <c r="P110" s="44"/>
+      <c r="Q110" s="45"/>
+      <c r="R110" s="45"/>
+      <c r="S110" s="46"/>
       <c r="T110" s="7"/>
       <c r="U110" s="7"/>
       <c r="V110" s="7"/>
@@ -5526,23 +5507,23 @@
     <row r="111" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
-      <c r="C111" s="43"/>
-      <c r="D111" s="44"/>
-      <c r="E111" s="45"/>
-      <c r="F111" s="43"/>
-      <c r="G111" s="44"/>
-      <c r="H111" s="45"/>
-      <c r="I111" s="43"/>
-      <c r="J111" s="44"/>
-      <c r="K111" s="44"/>
-      <c r="L111" s="45"/>
-      <c r="M111" s="43"/>
-      <c r="N111" s="44"/>
-      <c r="O111" s="45"/>
-      <c r="P111" s="43"/>
-      <c r="Q111" s="44"/>
-      <c r="R111" s="44"/>
-      <c r="S111" s="45"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="45"/>
+      <c r="E111" s="46"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="45"/>
+      <c r="H111" s="46"/>
+      <c r="I111" s="44"/>
+      <c r="J111" s="45"/>
+      <c r="K111" s="45"/>
+      <c r="L111" s="46"/>
+      <c r="M111" s="44"/>
+      <c r="N111" s="45"/>
+      <c r="O111" s="46"/>
+      <c r="P111" s="44"/>
+      <c r="Q111" s="45"/>
+      <c r="R111" s="45"/>
+      <c r="S111" s="46"/>
       <c r="T111" s="7"/>
       <c r="U111" s="7"/>
       <c r="V111" s="7"/>
@@ -5553,23 +5534,23 @@
     <row r="112" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
-      <c r="C112" s="43"/>
-      <c r="D112" s="44"/>
-      <c r="E112" s="45"/>
-      <c r="F112" s="43"/>
-      <c r="G112" s="44"/>
-      <c r="H112" s="45"/>
-      <c r="I112" s="43"/>
-      <c r="J112" s="44"/>
-      <c r="K112" s="44"/>
-      <c r="L112" s="45"/>
-      <c r="M112" s="43"/>
-      <c r="N112" s="44"/>
-      <c r="O112" s="45"/>
-      <c r="P112" s="43"/>
-      <c r="Q112" s="44"/>
-      <c r="R112" s="44"/>
-      <c r="S112" s="45"/>
+      <c r="C112" s="44"/>
+      <c r="D112" s="45"/>
+      <c r="E112" s="46"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="45"/>
+      <c r="H112" s="46"/>
+      <c r="I112" s="44"/>
+      <c r="J112" s="45"/>
+      <c r="K112" s="45"/>
+      <c r="L112" s="46"/>
+      <c r="M112" s="44"/>
+      <c r="N112" s="45"/>
+      <c r="O112" s="46"/>
+      <c r="P112" s="44"/>
+      <c r="Q112" s="45"/>
+      <c r="R112" s="45"/>
+      <c r="S112" s="46"/>
       <c r="T112" s="7"/>
       <c r="U112" s="7"/>
       <c r="V112" s="7"/>
@@ -5580,23 +5561,23 @@
     <row r="113" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
-      <c r="C113" s="43"/>
-      <c r="D113" s="44"/>
-      <c r="E113" s="45"/>
-      <c r="F113" s="43"/>
-      <c r="G113" s="44"/>
-      <c r="H113" s="45"/>
-      <c r="I113" s="43"/>
-      <c r="J113" s="44"/>
-      <c r="K113" s="44"/>
-      <c r="L113" s="45"/>
-      <c r="M113" s="43"/>
-      <c r="N113" s="44"/>
-      <c r="O113" s="45"/>
-      <c r="P113" s="43"/>
-      <c r="Q113" s="44"/>
-      <c r="R113" s="44"/>
-      <c r="S113" s="45"/>
+      <c r="C113" s="44"/>
+      <c r="D113" s="45"/>
+      <c r="E113" s="46"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="45"/>
+      <c r="H113" s="46"/>
+      <c r="I113" s="44"/>
+      <c r="J113" s="45"/>
+      <c r="K113" s="45"/>
+      <c r="L113" s="46"/>
+      <c r="M113" s="44"/>
+      <c r="N113" s="45"/>
+      <c r="O113" s="46"/>
+      <c r="P113" s="44"/>
+      <c r="Q113" s="45"/>
+      <c r="R113" s="45"/>
+      <c r="S113" s="46"/>
       <c r="T113" s="7"/>
       <c r="U113" s="7"/>
       <c r="V113" s="7"/>
@@ -5607,23 +5588,23 @@
     <row r="114" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
-      <c r="C114" s="43"/>
-      <c r="D114" s="44"/>
-      <c r="E114" s="45"/>
-      <c r="F114" s="43"/>
-      <c r="G114" s="44"/>
-      <c r="H114" s="45"/>
-      <c r="I114" s="43"/>
-      <c r="J114" s="44"/>
-      <c r="K114" s="44"/>
-      <c r="L114" s="45"/>
-      <c r="M114" s="43"/>
-      <c r="N114" s="44"/>
-      <c r="O114" s="45"/>
-      <c r="P114" s="43"/>
-      <c r="Q114" s="44"/>
-      <c r="R114" s="44"/>
-      <c r="S114" s="45"/>
+      <c r="C114" s="44"/>
+      <c r="D114" s="45"/>
+      <c r="E114" s="46"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="45"/>
+      <c r="H114" s="46"/>
+      <c r="I114" s="44"/>
+      <c r="J114" s="45"/>
+      <c r="K114" s="45"/>
+      <c r="L114" s="46"/>
+      <c r="M114" s="44"/>
+      <c r="N114" s="45"/>
+      <c r="O114" s="46"/>
+      <c r="P114" s="44"/>
+      <c r="Q114" s="45"/>
+      <c r="R114" s="45"/>
+      <c r="S114" s="46"/>
       <c r="T114" s="7"/>
       <c r="U114" s="7"/>
       <c r="V114" s="7"/>
@@ -5634,23 +5615,23 @@
     <row r="115" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
-      <c r="C115" s="43"/>
-      <c r="D115" s="44"/>
-      <c r="E115" s="45"/>
-      <c r="F115" s="43"/>
-      <c r="G115" s="44"/>
-      <c r="H115" s="45"/>
-      <c r="I115" s="43"/>
-      <c r="J115" s="44"/>
-      <c r="K115" s="44"/>
-      <c r="L115" s="45"/>
-      <c r="M115" s="43"/>
-      <c r="N115" s="44"/>
-      <c r="O115" s="45"/>
-      <c r="P115" s="43"/>
-      <c r="Q115" s="44"/>
-      <c r="R115" s="44"/>
-      <c r="S115" s="45"/>
+      <c r="C115" s="44"/>
+      <c r="D115" s="45"/>
+      <c r="E115" s="46"/>
+      <c r="F115" s="44"/>
+      <c r="G115" s="45"/>
+      <c r="H115" s="46"/>
+      <c r="I115" s="44"/>
+      <c r="J115" s="45"/>
+      <c r="K115" s="45"/>
+      <c r="L115" s="46"/>
+      <c r="M115" s="44"/>
+      <c r="N115" s="45"/>
+      <c r="O115" s="46"/>
+      <c r="P115" s="44"/>
+      <c r="Q115" s="45"/>
+      <c r="R115" s="45"/>
+      <c r="S115" s="46"/>
       <c r="T115" s="7"/>
       <c r="U115" s="7"/>
       <c r="V115" s="7"/>
@@ -5661,23 +5642,23 @@
     <row r="116" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
-      <c r="C116" s="43"/>
-      <c r="D116" s="44"/>
-      <c r="E116" s="45"/>
-      <c r="F116" s="43"/>
-      <c r="G116" s="44"/>
-      <c r="H116" s="45"/>
-      <c r="I116" s="43"/>
-      <c r="J116" s="44"/>
-      <c r="K116" s="44"/>
-      <c r="L116" s="45"/>
-      <c r="M116" s="43"/>
-      <c r="N116" s="44"/>
-      <c r="O116" s="45"/>
-      <c r="P116" s="43"/>
-      <c r="Q116" s="44"/>
-      <c r="R116" s="44"/>
-      <c r="S116" s="45"/>
+      <c r="C116" s="44"/>
+      <c r="D116" s="45"/>
+      <c r="E116" s="46"/>
+      <c r="F116" s="44"/>
+      <c r="G116" s="45"/>
+      <c r="H116" s="46"/>
+      <c r="I116" s="44"/>
+      <c r="J116" s="45"/>
+      <c r="K116" s="45"/>
+      <c r="L116" s="46"/>
+      <c r="M116" s="44"/>
+      <c r="N116" s="45"/>
+      <c r="O116" s="46"/>
+      <c r="P116" s="44"/>
+      <c r="Q116" s="45"/>
+      <c r="R116" s="45"/>
+      <c r="S116" s="46"/>
       <c r="T116" s="7"/>
       <c r="U116" s="7"/>
       <c r="V116" s="7"/>
@@ -5688,23 +5669,23 @@
     <row r="117" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
-      <c r="C117" s="43"/>
-      <c r="D117" s="44"/>
-      <c r="E117" s="45"/>
-      <c r="F117" s="43"/>
-      <c r="G117" s="44"/>
-      <c r="H117" s="45"/>
-      <c r="I117" s="43"/>
-      <c r="J117" s="44"/>
-      <c r="K117" s="44"/>
-      <c r="L117" s="45"/>
-      <c r="M117" s="43"/>
-      <c r="N117" s="44"/>
-      <c r="O117" s="45"/>
-      <c r="P117" s="43"/>
-      <c r="Q117" s="44"/>
-      <c r="R117" s="44"/>
-      <c r="S117" s="45"/>
+      <c r="C117" s="44"/>
+      <c r="D117" s="45"/>
+      <c r="E117" s="46"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="45"/>
+      <c r="H117" s="46"/>
+      <c r="I117" s="44"/>
+      <c r="J117" s="45"/>
+      <c r="K117" s="45"/>
+      <c r="L117" s="46"/>
+      <c r="M117" s="44"/>
+      <c r="N117" s="45"/>
+      <c r="O117" s="46"/>
+      <c r="P117" s="44"/>
+      <c r="Q117" s="45"/>
+      <c r="R117" s="45"/>
+      <c r="S117" s="46"/>
       <c r="T117" s="7"/>
       <c r="U117" s="7"/>
       <c r="V117" s="7"/>
@@ -5715,23 +5696,23 @@
     <row r="118" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
-      <c r="C118" s="43"/>
-      <c r="D118" s="44"/>
-      <c r="E118" s="45"/>
-      <c r="F118" s="43"/>
-      <c r="G118" s="44"/>
-      <c r="H118" s="45"/>
-      <c r="I118" s="43"/>
-      <c r="J118" s="44"/>
-      <c r="K118" s="44"/>
-      <c r="L118" s="45"/>
-      <c r="M118" s="43"/>
-      <c r="N118" s="44"/>
-      <c r="O118" s="45"/>
-      <c r="P118" s="43"/>
-      <c r="Q118" s="44"/>
-      <c r="R118" s="44"/>
-      <c r="S118" s="45"/>
+      <c r="C118" s="44"/>
+      <c r="D118" s="45"/>
+      <c r="E118" s="46"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="45"/>
+      <c r="H118" s="46"/>
+      <c r="I118" s="44"/>
+      <c r="J118" s="45"/>
+      <c r="K118" s="45"/>
+      <c r="L118" s="46"/>
+      <c r="M118" s="44"/>
+      <c r="N118" s="45"/>
+      <c r="O118" s="46"/>
+      <c r="P118" s="44"/>
+      <c r="Q118" s="45"/>
+      <c r="R118" s="45"/>
+      <c r="S118" s="46"/>
       <c r="T118" s="7"/>
       <c r="U118" s="7"/>
       <c r="V118" s="7"/>
@@ -5742,23 +5723,23 @@
     <row r="119" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
-      <c r="C119" s="43"/>
-      <c r="D119" s="44"/>
-      <c r="E119" s="45"/>
-      <c r="F119" s="43"/>
-      <c r="G119" s="44"/>
-      <c r="H119" s="45"/>
-      <c r="I119" s="43"/>
-      <c r="J119" s="44"/>
-      <c r="K119" s="44"/>
-      <c r="L119" s="45"/>
-      <c r="M119" s="43"/>
-      <c r="N119" s="44"/>
-      <c r="O119" s="45"/>
-      <c r="P119" s="43"/>
-      <c r="Q119" s="44"/>
-      <c r="R119" s="44"/>
-      <c r="S119" s="45"/>
+      <c r="C119" s="44"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="46"/>
+      <c r="F119" s="44"/>
+      <c r="G119" s="45"/>
+      <c r="H119" s="46"/>
+      <c r="I119" s="44"/>
+      <c r="J119" s="45"/>
+      <c r="K119" s="45"/>
+      <c r="L119" s="46"/>
+      <c r="M119" s="44"/>
+      <c r="N119" s="45"/>
+      <c r="O119" s="46"/>
+      <c r="P119" s="44"/>
+      <c r="Q119" s="45"/>
+      <c r="R119" s="45"/>
+      <c r="S119" s="46"/>
       <c r="T119" s="7"/>
       <c r="U119" s="7"/>
       <c r="V119" s="7"/>
@@ -5769,23 +5750,23 @@
     <row r="120" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
-      <c r="C120" s="43"/>
-      <c r="D120" s="44"/>
-      <c r="E120" s="45"/>
-      <c r="F120" s="43"/>
-      <c r="G120" s="44"/>
-      <c r="H120" s="45"/>
-      <c r="I120" s="43"/>
-      <c r="J120" s="44"/>
-      <c r="K120" s="44"/>
-      <c r="L120" s="45"/>
-      <c r="M120" s="43"/>
-      <c r="N120" s="44"/>
-      <c r="O120" s="45"/>
-      <c r="P120" s="43"/>
-      <c r="Q120" s="44"/>
-      <c r="R120" s="44"/>
-      <c r="S120" s="45"/>
+      <c r="C120" s="44"/>
+      <c r="D120" s="45"/>
+      <c r="E120" s="46"/>
+      <c r="F120" s="44"/>
+      <c r="G120" s="45"/>
+      <c r="H120" s="46"/>
+      <c r="I120" s="44"/>
+      <c r="J120" s="45"/>
+      <c r="K120" s="45"/>
+      <c r="L120" s="46"/>
+      <c r="M120" s="44"/>
+      <c r="N120" s="45"/>
+      <c r="O120" s="46"/>
+      <c r="P120" s="44"/>
+      <c r="Q120" s="45"/>
+      <c r="R120" s="45"/>
+      <c r="S120" s="46"/>
       <c r="T120" s="7"/>
       <c r="U120" s="7"/>
       <c r="V120" s="7"/>
@@ -5796,23 +5777,23 @@
     <row r="121" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
-      <c r="C121" s="43"/>
-      <c r="D121" s="44"/>
-      <c r="E121" s="45"/>
-      <c r="F121" s="43"/>
-      <c r="G121" s="44"/>
-      <c r="H121" s="45"/>
-      <c r="I121" s="43"/>
-      <c r="J121" s="44"/>
-      <c r="K121" s="44"/>
-      <c r="L121" s="45"/>
-      <c r="M121" s="43"/>
-      <c r="N121" s="44"/>
-      <c r="O121" s="45"/>
-      <c r="P121" s="43"/>
-      <c r="Q121" s="44"/>
-      <c r="R121" s="44"/>
-      <c r="S121" s="45"/>
+      <c r="C121" s="44"/>
+      <c r="D121" s="45"/>
+      <c r="E121" s="46"/>
+      <c r="F121" s="44"/>
+      <c r="G121" s="45"/>
+      <c r="H121" s="46"/>
+      <c r="I121" s="44"/>
+      <c r="J121" s="45"/>
+      <c r="K121" s="45"/>
+      <c r="L121" s="46"/>
+      <c r="M121" s="44"/>
+      <c r="N121" s="45"/>
+      <c r="O121" s="46"/>
+      <c r="P121" s="44"/>
+      <c r="Q121" s="45"/>
+      <c r="R121" s="45"/>
+      <c r="S121" s="46"/>
       <c r="T121" s="7"/>
       <c r="U121" s="7"/>
       <c r="V121" s="7"/>
@@ -5823,23 +5804,23 @@
     <row r="122" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
-      <c r="C122" s="43"/>
-      <c r="D122" s="44"/>
-      <c r="E122" s="45"/>
-      <c r="F122" s="43"/>
-      <c r="G122" s="44"/>
-      <c r="H122" s="45"/>
-      <c r="I122" s="43"/>
-      <c r="J122" s="44"/>
-      <c r="K122" s="44"/>
-      <c r="L122" s="45"/>
-      <c r="M122" s="43"/>
-      <c r="N122" s="44"/>
-      <c r="O122" s="45"/>
-      <c r="P122" s="43"/>
-      <c r="Q122" s="44"/>
-      <c r="R122" s="44"/>
-      <c r="S122" s="45"/>
+      <c r="C122" s="44"/>
+      <c r="D122" s="45"/>
+      <c r="E122" s="46"/>
+      <c r="F122" s="44"/>
+      <c r="G122" s="45"/>
+      <c r="H122" s="46"/>
+      <c r="I122" s="44"/>
+      <c r="J122" s="45"/>
+      <c r="K122" s="45"/>
+      <c r="L122" s="46"/>
+      <c r="M122" s="44"/>
+      <c r="N122" s="45"/>
+      <c r="O122" s="46"/>
+      <c r="P122" s="44"/>
+      <c r="Q122" s="45"/>
+      <c r="R122" s="45"/>
+      <c r="S122" s="46"/>
       <c r="T122" s="7"/>
       <c r="U122" s="7"/>
       <c r="V122" s="7"/>
@@ -5850,23 +5831,23 @@
     <row r="123" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
-      <c r="C123" s="43"/>
-      <c r="D123" s="44"/>
-      <c r="E123" s="45"/>
-      <c r="F123" s="43"/>
-      <c r="G123" s="44"/>
-      <c r="H123" s="45"/>
-      <c r="I123" s="43"/>
-      <c r="J123" s="44"/>
-      <c r="K123" s="44"/>
-      <c r="L123" s="45"/>
-      <c r="M123" s="43"/>
-      <c r="N123" s="44"/>
-      <c r="O123" s="45"/>
-      <c r="P123" s="43"/>
-      <c r="Q123" s="44"/>
-      <c r="R123" s="44"/>
-      <c r="S123" s="45"/>
+      <c r="C123" s="44"/>
+      <c r="D123" s="45"/>
+      <c r="E123" s="46"/>
+      <c r="F123" s="44"/>
+      <c r="G123" s="45"/>
+      <c r="H123" s="46"/>
+      <c r="I123" s="44"/>
+      <c r="J123" s="45"/>
+      <c r="K123" s="45"/>
+      <c r="L123" s="46"/>
+      <c r="M123" s="44"/>
+      <c r="N123" s="45"/>
+      <c r="O123" s="46"/>
+      <c r="P123" s="44"/>
+      <c r="Q123" s="45"/>
+      <c r="R123" s="45"/>
+      <c r="S123" s="46"/>
       <c r="T123" s="7"/>
       <c r="U123" s="7"/>
       <c r="V123" s="7"/>
@@ -5877,23 +5858,23 @@
     <row r="124" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
-      <c r="C124" s="43"/>
-      <c r="D124" s="44"/>
-      <c r="E124" s="45"/>
-      <c r="F124" s="43"/>
-      <c r="G124" s="44"/>
-      <c r="H124" s="45"/>
-      <c r="I124" s="43"/>
-      <c r="J124" s="44"/>
-      <c r="K124" s="44"/>
-      <c r="L124" s="45"/>
-      <c r="M124" s="43"/>
-      <c r="N124" s="44"/>
-      <c r="O124" s="45"/>
-      <c r="P124" s="43"/>
-      <c r="Q124" s="44"/>
-      <c r="R124" s="44"/>
-      <c r="S124" s="45"/>
+      <c r="C124" s="44"/>
+      <c r="D124" s="45"/>
+      <c r="E124" s="46"/>
+      <c r="F124" s="44"/>
+      <c r="G124" s="45"/>
+      <c r="H124" s="46"/>
+      <c r="I124" s="44"/>
+      <c r="J124" s="45"/>
+      <c r="K124" s="45"/>
+      <c r="L124" s="46"/>
+      <c r="M124" s="44"/>
+      <c r="N124" s="45"/>
+      <c r="O124" s="46"/>
+      <c r="P124" s="44"/>
+      <c r="Q124" s="45"/>
+      <c r="R124" s="45"/>
+      <c r="S124" s="46"/>
       <c r="T124" s="7"/>
       <c r="U124" s="7"/>
       <c r="V124" s="7"/>
@@ -5904,23 +5885,23 @@
     <row r="125" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
-      <c r="C125" s="43"/>
-      <c r="D125" s="44"/>
-      <c r="E125" s="45"/>
-      <c r="F125" s="43"/>
-      <c r="G125" s="44"/>
-      <c r="H125" s="45"/>
-      <c r="I125" s="43"/>
-      <c r="J125" s="44"/>
-      <c r="K125" s="44"/>
-      <c r="L125" s="45"/>
-      <c r="M125" s="43"/>
-      <c r="N125" s="44"/>
-      <c r="O125" s="45"/>
-      <c r="P125" s="43"/>
-      <c r="Q125" s="44"/>
-      <c r="R125" s="44"/>
-      <c r="S125" s="45"/>
+      <c r="C125" s="44"/>
+      <c r="D125" s="45"/>
+      <c r="E125" s="46"/>
+      <c r="F125" s="44"/>
+      <c r="G125" s="45"/>
+      <c r="H125" s="46"/>
+      <c r="I125" s="44"/>
+      <c r="J125" s="45"/>
+      <c r="K125" s="45"/>
+      <c r="L125" s="46"/>
+      <c r="M125" s="44"/>
+      <c r="N125" s="45"/>
+      <c r="O125" s="46"/>
+      <c r="P125" s="44"/>
+      <c r="Q125" s="45"/>
+      <c r="R125" s="45"/>
+      <c r="S125" s="46"/>
       <c r="T125" s="7"/>
       <c r="U125" s="7"/>
       <c r="V125" s="7"/>
@@ -5931,23 +5912,23 @@
     <row r="126" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
-      <c r="C126" s="43"/>
-      <c r="D126" s="44"/>
-      <c r="E126" s="45"/>
-      <c r="F126" s="43"/>
-      <c r="G126" s="44"/>
-      <c r="H126" s="45"/>
-      <c r="I126" s="43"/>
-      <c r="J126" s="44"/>
-      <c r="K126" s="44"/>
-      <c r="L126" s="45"/>
-      <c r="M126" s="43"/>
-      <c r="N126" s="44"/>
-      <c r="O126" s="45"/>
-      <c r="P126" s="43"/>
-      <c r="Q126" s="44"/>
-      <c r="R126" s="44"/>
-      <c r="S126" s="45"/>
+      <c r="C126" s="44"/>
+      <c r="D126" s="45"/>
+      <c r="E126" s="46"/>
+      <c r="F126" s="44"/>
+      <c r="G126" s="45"/>
+      <c r="H126" s="46"/>
+      <c r="I126" s="44"/>
+      <c r="J126" s="45"/>
+      <c r="K126" s="45"/>
+      <c r="L126" s="46"/>
+      <c r="M126" s="44"/>
+      <c r="N126" s="45"/>
+      <c r="O126" s="46"/>
+      <c r="P126" s="44"/>
+      <c r="Q126" s="45"/>
+      <c r="R126" s="45"/>
+      <c r="S126" s="46"/>
       <c r="T126" s="7"/>
       <c r="U126" s="7"/>
       <c r="V126" s="7"/>
@@ -5958,23 +5939,23 @@
     <row r="127" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
-      <c r="C127" s="43"/>
-      <c r="D127" s="44"/>
-      <c r="E127" s="45"/>
-      <c r="F127" s="43"/>
-      <c r="G127" s="44"/>
-      <c r="H127" s="45"/>
-      <c r="I127" s="43"/>
-      <c r="J127" s="44"/>
-      <c r="K127" s="44"/>
-      <c r="L127" s="45"/>
-      <c r="M127" s="43"/>
-      <c r="N127" s="44"/>
-      <c r="O127" s="45"/>
-      <c r="P127" s="43"/>
-      <c r="Q127" s="44"/>
-      <c r="R127" s="44"/>
-      <c r="S127" s="45"/>
+      <c r="C127" s="44"/>
+      <c r="D127" s="45"/>
+      <c r="E127" s="46"/>
+      <c r="F127" s="44"/>
+      <c r="G127" s="45"/>
+      <c r="H127" s="46"/>
+      <c r="I127" s="44"/>
+      <c r="J127" s="45"/>
+      <c r="K127" s="45"/>
+      <c r="L127" s="46"/>
+      <c r="M127" s="44"/>
+      <c r="N127" s="45"/>
+      <c r="O127" s="46"/>
+      <c r="P127" s="44"/>
+      <c r="Q127" s="45"/>
+      <c r="R127" s="45"/>
+      <c r="S127" s="46"/>
       <c r="T127" s="7"/>
       <c r="U127" s="7"/>
       <c r="V127" s="7"/>
@@ -5985,23 +5966,23 @@
     <row r="128" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
-      <c r="C128" s="43"/>
-      <c r="D128" s="44"/>
-      <c r="E128" s="45"/>
-      <c r="F128" s="43"/>
-      <c r="G128" s="44"/>
-      <c r="H128" s="45"/>
-      <c r="I128" s="43"/>
-      <c r="J128" s="44"/>
-      <c r="K128" s="44"/>
-      <c r="L128" s="45"/>
-      <c r="M128" s="43"/>
-      <c r="N128" s="44"/>
-      <c r="O128" s="45"/>
-      <c r="P128" s="43"/>
-      <c r="Q128" s="44"/>
-      <c r="R128" s="44"/>
-      <c r="S128" s="45"/>
+      <c r="C128" s="44"/>
+      <c r="D128" s="45"/>
+      <c r="E128" s="46"/>
+      <c r="F128" s="44"/>
+      <c r="G128" s="45"/>
+      <c r="H128" s="46"/>
+      <c r="I128" s="44"/>
+      <c r="J128" s="45"/>
+      <c r="K128" s="45"/>
+      <c r="L128" s="46"/>
+      <c r="M128" s="44"/>
+      <c r="N128" s="45"/>
+      <c r="O128" s="46"/>
+      <c r="P128" s="44"/>
+      <c r="Q128" s="45"/>
+      <c r="R128" s="45"/>
+      <c r="S128" s="46"/>
       <c r="T128" s="7"/>
       <c r="U128" s="7"/>
       <c r="V128" s="7"/>
@@ -6012,23 +5993,23 @@
     <row r="129" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
-      <c r="C129" s="43"/>
-      <c r="D129" s="44"/>
-      <c r="E129" s="45"/>
-      <c r="F129" s="43"/>
-      <c r="G129" s="44"/>
-      <c r="H129" s="45"/>
-      <c r="I129" s="43"/>
-      <c r="J129" s="44"/>
-      <c r="K129" s="44"/>
-      <c r="L129" s="45"/>
-      <c r="M129" s="43"/>
-      <c r="N129" s="44"/>
-      <c r="O129" s="45"/>
-      <c r="P129" s="43"/>
-      <c r="Q129" s="44"/>
-      <c r="R129" s="44"/>
-      <c r="S129" s="45"/>
+      <c r="C129" s="44"/>
+      <c r="D129" s="45"/>
+      <c r="E129" s="46"/>
+      <c r="F129" s="44"/>
+      <c r="G129" s="45"/>
+      <c r="H129" s="46"/>
+      <c r="I129" s="44"/>
+      <c r="J129" s="45"/>
+      <c r="K129" s="45"/>
+      <c r="L129" s="46"/>
+      <c r="M129" s="44"/>
+      <c r="N129" s="45"/>
+      <c r="O129" s="46"/>
+      <c r="P129" s="44"/>
+      <c r="Q129" s="45"/>
+      <c r="R129" s="45"/>
+      <c r="S129" s="46"/>
       <c r="T129" s="7"/>
       <c r="U129" s="7"/>
       <c r="V129" s="7"/>
@@ -6039,23 +6020,23 @@
     <row r="130" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
-      <c r="C130" s="43"/>
-      <c r="D130" s="44"/>
-      <c r="E130" s="45"/>
-      <c r="F130" s="43"/>
-      <c r="G130" s="44"/>
-      <c r="H130" s="45"/>
-      <c r="I130" s="43"/>
-      <c r="J130" s="44"/>
-      <c r="K130" s="44"/>
-      <c r="L130" s="45"/>
-      <c r="M130" s="43"/>
-      <c r="N130" s="44"/>
-      <c r="O130" s="45"/>
-      <c r="P130" s="43"/>
-      <c r="Q130" s="44"/>
-      <c r="R130" s="44"/>
-      <c r="S130" s="45"/>
+      <c r="C130" s="44"/>
+      <c r="D130" s="45"/>
+      <c r="E130" s="46"/>
+      <c r="F130" s="44"/>
+      <c r="G130" s="45"/>
+      <c r="H130" s="46"/>
+      <c r="I130" s="44"/>
+      <c r="J130" s="45"/>
+      <c r="K130" s="45"/>
+      <c r="L130" s="46"/>
+      <c r="M130" s="44"/>
+      <c r="N130" s="45"/>
+      <c r="O130" s="46"/>
+      <c r="P130" s="44"/>
+      <c r="Q130" s="45"/>
+      <c r="R130" s="45"/>
+      <c r="S130" s="46"/>
       <c r="T130" s="7"/>
       <c r="U130" s="7"/>
       <c r="V130" s="7"/>
@@ -6066,23 +6047,23 @@
     <row r="131" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
-      <c r="C131" s="43"/>
-      <c r="D131" s="44"/>
-      <c r="E131" s="45"/>
-      <c r="F131" s="43"/>
-      <c r="G131" s="44"/>
-      <c r="H131" s="45"/>
-      <c r="I131" s="43"/>
-      <c r="J131" s="44"/>
-      <c r="K131" s="44"/>
-      <c r="L131" s="45"/>
-      <c r="M131" s="43"/>
-      <c r="N131" s="44"/>
-      <c r="O131" s="45"/>
-      <c r="P131" s="43"/>
-      <c r="Q131" s="44"/>
-      <c r="R131" s="44"/>
-      <c r="S131" s="45"/>
+      <c r="C131" s="44"/>
+      <c r="D131" s="45"/>
+      <c r="E131" s="46"/>
+      <c r="F131" s="44"/>
+      <c r="G131" s="45"/>
+      <c r="H131" s="46"/>
+      <c r="I131" s="44"/>
+      <c r="J131" s="45"/>
+      <c r="K131" s="45"/>
+      <c r="L131" s="46"/>
+      <c r="M131" s="44"/>
+      <c r="N131" s="45"/>
+      <c r="O131" s="46"/>
+      <c r="P131" s="44"/>
+      <c r="Q131" s="45"/>
+      <c r="R131" s="45"/>
+      <c r="S131" s="46"/>
       <c r="T131" s="7"/>
       <c r="U131" s="7"/>
       <c r="V131" s="7"/>
@@ -6093,23 +6074,23 @@
     <row r="132" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
-      <c r="C132" s="43"/>
-      <c r="D132" s="44"/>
-      <c r="E132" s="45"/>
-      <c r="F132" s="43"/>
-      <c r="G132" s="44"/>
-      <c r="H132" s="45"/>
-      <c r="I132" s="43"/>
-      <c r="J132" s="44"/>
-      <c r="K132" s="44"/>
-      <c r="L132" s="45"/>
-      <c r="M132" s="43"/>
-      <c r="N132" s="44"/>
-      <c r="O132" s="45"/>
-      <c r="P132" s="43"/>
-      <c r="Q132" s="44"/>
-      <c r="R132" s="44"/>
-      <c r="S132" s="45"/>
+      <c r="C132" s="44"/>
+      <c r="D132" s="45"/>
+      <c r="E132" s="46"/>
+      <c r="F132" s="44"/>
+      <c r="G132" s="45"/>
+      <c r="H132" s="46"/>
+      <c r="I132" s="44"/>
+      <c r="J132" s="45"/>
+      <c r="K132" s="45"/>
+      <c r="L132" s="46"/>
+      <c r="M132" s="44"/>
+      <c r="N132" s="45"/>
+      <c r="O132" s="46"/>
+      <c r="P132" s="44"/>
+      <c r="Q132" s="45"/>
+      <c r="R132" s="45"/>
+      <c r="S132" s="46"/>
       <c r="T132" s="7"/>
       <c r="U132" s="7"/>
       <c r="V132" s="7"/>
@@ -6120,23 +6101,23 @@
     <row r="133" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
-      <c r="C133" s="43"/>
-      <c r="D133" s="44"/>
-      <c r="E133" s="45"/>
-      <c r="F133" s="43"/>
-      <c r="G133" s="44"/>
-      <c r="H133" s="45"/>
-      <c r="I133" s="43"/>
-      <c r="J133" s="44"/>
-      <c r="K133" s="44"/>
-      <c r="L133" s="45"/>
-      <c r="M133" s="43"/>
-      <c r="N133" s="44"/>
-      <c r="O133" s="45"/>
-      <c r="P133" s="43"/>
-      <c r="Q133" s="44"/>
-      <c r="R133" s="44"/>
-      <c r="S133" s="45"/>
+      <c r="C133" s="44"/>
+      <c r="D133" s="45"/>
+      <c r="E133" s="46"/>
+      <c r="F133" s="44"/>
+      <c r="G133" s="45"/>
+      <c r="H133" s="46"/>
+      <c r="I133" s="44"/>
+      <c r="J133" s="45"/>
+      <c r="K133" s="45"/>
+      <c r="L133" s="46"/>
+      <c r="M133" s="44"/>
+      <c r="N133" s="45"/>
+      <c r="O133" s="46"/>
+      <c r="P133" s="44"/>
+      <c r="Q133" s="45"/>
+      <c r="R133" s="45"/>
+      <c r="S133" s="46"/>
       <c r="T133" s="7"/>
       <c r="U133" s="7"/>
       <c r="V133" s="7"/>
@@ -6147,23 +6128,23 @@
     <row r="134" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
-      <c r="C134" s="43"/>
-      <c r="D134" s="44"/>
-      <c r="E134" s="45"/>
-      <c r="F134" s="43"/>
-      <c r="G134" s="44"/>
-      <c r="H134" s="45"/>
-      <c r="I134" s="43"/>
-      <c r="J134" s="44"/>
-      <c r="K134" s="44"/>
-      <c r="L134" s="45"/>
-      <c r="M134" s="43"/>
-      <c r="N134" s="44"/>
-      <c r="O134" s="45"/>
-      <c r="P134" s="43"/>
-      <c r="Q134" s="44"/>
-      <c r="R134" s="44"/>
-      <c r="S134" s="45"/>
+      <c r="C134" s="44"/>
+      <c r="D134" s="45"/>
+      <c r="E134" s="46"/>
+      <c r="F134" s="44"/>
+      <c r="G134" s="45"/>
+      <c r="H134" s="46"/>
+      <c r="I134" s="44"/>
+      <c r="J134" s="45"/>
+      <c r="K134" s="45"/>
+      <c r="L134" s="46"/>
+      <c r="M134" s="44"/>
+      <c r="N134" s="45"/>
+      <c r="O134" s="46"/>
+      <c r="P134" s="44"/>
+      <c r="Q134" s="45"/>
+      <c r="R134" s="45"/>
+      <c r="S134" s="46"/>
       <c r="T134" s="7"/>
       <c r="U134" s="7"/>
       <c r="V134" s="7"/>
@@ -6174,23 +6155,23 @@
     <row r="135" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
-      <c r="C135" s="43"/>
-      <c r="D135" s="44"/>
-      <c r="E135" s="45"/>
-      <c r="F135" s="43"/>
-      <c r="G135" s="44"/>
-      <c r="H135" s="45"/>
-      <c r="I135" s="43"/>
-      <c r="J135" s="44"/>
-      <c r="K135" s="44"/>
-      <c r="L135" s="45"/>
-      <c r="M135" s="43"/>
-      <c r="N135" s="44"/>
-      <c r="O135" s="45"/>
-      <c r="P135" s="43"/>
-      <c r="Q135" s="44"/>
-      <c r="R135" s="44"/>
-      <c r="S135" s="45"/>
+      <c r="C135" s="44"/>
+      <c r="D135" s="45"/>
+      <c r="E135" s="46"/>
+      <c r="F135" s="44"/>
+      <c r="G135" s="45"/>
+      <c r="H135" s="46"/>
+      <c r="I135" s="44"/>
+      <c r="J135" s="45"/>
+      <c r="K135" s="45"/>
+      <c r="L135" s="46"/>
+      <c r="M135" s="44"/>
+      <c r="N135" s="45"/>
+      <c r="O135" s="46"/>
+      <c r="P135" s="44"/>
+      <c r="Q135" s="45"/>
+      <c r="R135" s="45"/>
+      <c r="S135" s="46"/>
       <c r="T135" s="7"/>
       <c r="U135" s="7"/>
       <c r="V135" s="7"/>
@@ -6201,23 +6182,23 @@
     <row r="136" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
-      <c r="C136" s="43"/>
-      <c r="D136" s="44"/>
-      <c r="E136" s="45"/>
-      <c r="F136" s="43"/>
-      <c r="G136" s="44"/>
-      <c r="H136" s="45"/>
-      <c r="I136" s="43"/>
-      <c r="J136" s="44"/>
-      <c r="K136" s="44"/>
-      <c r="L136" s="45"/>
-      <c r="M136" s="43"/>
-      <c r="N136" s="44"/>
-      <c r="O136" s="45"/>
-      <c r="P136" s="43"/>
-      <c r="Q136" s="44"/>
-      <c r="R136" s="44"/>
-      <c r="S136" s="45"/>
+      <c r="C136" s="44"/>
+      <c r="D136" s="45"/>
+      <c r="E136" s="46"/>
+      <c r="F136" s="44"/>
+      <c r="G136" s="45"/>
+      <c r="H136" s="46"/>
+      <c r="I136" s="44"/>
+      <c r="J136" s="45"/>
+      <c r="K136" s="45"/>
+      <c r="L136" s="46"/>
+      <c r="M136" s="44"/>
+      <c r="N136" s="45"/>
+      <c r="O136" s="46"/>
+      <c r="P136" s="44"/>
+      <c r="Q136" s="45"/>
+      <c r="R136" s="45"/>
+      <c r="S136" s="46"/>
       <c r="T136" s="7"/>
       <c r="U136" s="7"/>
       <c r="V136" s="7"/>
@@ -6228,23 +6209,23 @@
     <row r="137" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
-      <c r="C137" s="43"/>
-      <c r="D137" s="44"/>
-      <c r="E137" s="45"/>
-      <c r="F137" s="43"/>
-      <c r="G137" s="44"/>
-      <c r="H137" s="45"/>
-      <c r="I137" s="43"/>
-      <c r="J137" s="44"/>
-      <c r="K137" s="44"/>
-      <c r="L137" s="45"/>
-      <c r="M137" s="43"/>
-      <c r="N137" s="44"/>
-      <c r="O137" s="45"/>
-      <c r="P137" s="43"/>
-      <c r="Q137" s="44"/>
-      <c r="R137" s="44"/>
-      <c r="S137" s="45"/>
+      <c r="C137" s="44"/>
+      <c r="D137" s="45"/>
+      <c r="E137" s="46"/>
+      <c r="F137" s="44"/>
+      <c r="G137" s="45"/>
+      <c r="H137" s="46"/>
+      <c r="I137" s="44"/>
+      <c r="J137" s="45"/>
+      <c r="K137" s="45"/>
+      <c r="L137" s="46"/>
+      <c r="M137" s="44"/>
+      <c r="N137" s="45"/>
+      <c r="O137" s="46"/>
+      <c r="P137" s="44"/>
+      <c r="Q137" s="45"/>
+      <c r="R137" s="45"/>
+      <c r="S137" s="46"/>
       <c r="T137" s="7"/>
       <c r="U137" s="7"/>
       <c r="V137" s="7"/>
@@ -6255,23 +6236,23 @@
     <row r="138" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
-      <c r="C138" s="43"/>
-      <c r="D138" s="44"/>
-      <c r="E138" s="45"/>
-      <c r="F138" s="43"/>
-      <c r="G138" s="44"/>
-      <c r="H138" s="45"/>
-      <c r="I138" s="43"/>
-      <c r="J138" s="44"/>
-      <c r="K138" s="44"/>
-      <c r="L138" s="45"/>
-      <c r="M138" s="43"/>
-      <c r="N138" s="44"/>
-      <c r="O138" s="45"/>
-      <c r="P138" s="43"/>
-      <c r="Q138" s="44"/>
-      <c r="R138" s="44"/>
-      <c r="S138" s="45"/>
+      <c r="C138" s="44"/>
+      <c r="D138" s="45"/>
+      <c r="E138" s="46"/>
+      <c r="F138" s="44"/>
+      <c r="G138" s="45"/>
+      <c r="H138" s="46"/>
+      <c r="I138" s="44"/>
+      <c r="J138" s="45"/>
+      <c r="K138" s="45"/>
+      <c r="L138" s="46"/>
+      <c r="M138" s="44"/>
+      <c r="N138" s="45"/>
+      <c r="O138" s="46"/>
+      <c r="P138" s="44"/>
+      <c r="Q138" s="45"/>
+      <c r="R138" s="45"/>
+      <c r="S138" s="46"/>
       <c r="T138" s="7"/>
       <c r="U138" s="7"/>
       <c r="V138" s="7"/>
@@ -6282,23 +6263,23 @@
     <row r="139" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
-      <c r="C139" s="43"/>
-      <c r="D139" s="44"/>
-      <c r="E139" s="45"/>
-      <c r="F139" s="43"/>
-      <c r="G139" s="44"/>
-      <c r="H139" s="45"/>
-      <c r="I139" s="43"/>
-      <c r="J139" s="44"/>
-      <c r="K139" s="44"/>
-      <c r="L139" s="45"/>
-      <c r="M139" s="43"/>
-      <c r="N139" s="44"/>
-      <c r="O139" s="45"/>
-      <c r="P139" s="43"/>
-      <c r="Q139" s="44"/>
-      <c r="R139" s="44"/>
-      <c r="S139" s="45"/>
+      <c r="C139" s="44"/>
+      <c r="D139" s="45"/>
+      <c r="E139" s="46"/>
+      <c r="F139" s="44"/>
+      <c r="G139" s="45"/>
+      <c r="H139" s="46"/>
+      <c r="I139" s="44"/>
+      <c r="J139" s="45"/>
+      <c r="K139" s="45"/>
+      <c r="L139" s="46"/>
+      <c r="M139" s="44"/>
+      <c r="N139" s="45"/>
+      <c r="O139" s="46"/>
+      <c r="P139" s="44"/>
+      <c r="Q139" s="45"/>
+      <c r="R139" s="45"/>
+      <c r="S139" s="46"/>
       <c r="T139" s="7"/>
       <c r="U139" s="7"/>
       <c r="V139" s="7"/>
@@ -6309,23 +6290,23 @@
     <row r="140" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
-      <c r="C140" s="43"/>
-      <c r="D140" s="44"/>
-      <c r="E140" s="45"/>
-      <c r="F140" s="43"/>
-      <c r="G140" s="44"/>
-      <c r="H140" s="45"/>
-      <c r="I140" s="43"/>
-      <c r="J140" s="44"/>
-      <c r="K140" s="44"/>
-      <c r="L140" s="45"/>
-      <c r="M140" s="43"/>
-      <c r="N140" s="44"/>
-      <c r="O140" s="45"/>
-      <c r="P140" s="43"/>
-      <c r="Q140" s="44"/>
-      <c r="R140" s="44"/>
-      <c r="S140" s="45"/>
+      <c r="C140" s="44"/>
+      <c r="D140" s="45"/>
+      <c r="E140" s="46"/>
+      <c r="F140" s="44"/>
+      <c r="G140" s="45"/>
+      <c r="H140" s="46"/>
+      <c r="I140" s="44"/>
+      <c r="J140" s="45"/>
+      <c r="K140" s="45"/>
+      <c r="L140" s="46"/>
+      <c r="M140" s="44"/>
+      <c r="N140" s="45"/>
+      <c r="O140" s="46"/>
+      <c r="P140" s="44"/>
+      <c r="Q140" s="45"/>
+      <c r="R140" s="45"/>
+      <c r="S140" s="46"/>
       <c r="T140" s="7"/>
       <c r="U140" s="7"/>
       <c r="V140" s="7"/>
@@ -6336,23 +6317,23 @@
     <row r="141" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
-      <c r="C141" s="43"/>
-      <c r="D141" s="44"/>
-      <c r="E141" s="45"/>
-      <c r="F141" s="43"/>
-      <c r="G141" s="44"/>
-      <c r="H141" s="45"/>
-      <c r="I141" s="43"/>
-      <c r="J141" s="44"/>
-      <c r="K141" s="44"/>
-      <c r="L141" s="45"/>
-      <c r="M141" s="43"/>
-      <c r="N141" s="44"/>
-      <c r="O141" s="45"/>
-      <c r="P141" s="43"/>
-      <c r="Q141" s="44"/>
-      <c r="R141" s="44"/>
-      <c r="S141" s="45"/>
+      <c r="C141" s="44"/>
+      <c r="D141" s="45"/>
+      <c r="E141" s="46"/>
+      <c r="F141" s="44"/>
+      <c r="G141" s="45"/>
+      <c r="H141" s="46"/>
+      <c r="I141" s="44"/>
+      <c r="J141" s="45"/>
+      <c r="K141" s="45"/>
+      <c r="L141" s="46"/>
+      <c r="M141" s="44"/>
+      <c r="N141" s="45"/>
+      <c r="O141" s="46"/>
+      <c r="P141" s="44"/>
+      <c r="Q141" s="45"/>
+      <c r="R141" s="45"/>
+      <c r="S141" s="46"/>
       <c r="T141" s="7"/>
       <c r="U141" s="7"/>
       <c r="V141" s="7"/>
@@ -6363,23 +6344,23 @@
     <row r="142" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
-      <c r="C142" s="43"/>
-      <c r="D142" s="44"/>
-      <c r="E142" s="45"/>
-      <c r="F142" s="43"/>
-      <c r="G142" s="44"/>
-      <c r="H142" s="45"/>
-      <c r="I142" s="43"/>
-      <c r="J142" s="44"/>
-      <c r="K142" s="44"/>
-      <c r="L142" s="45"/>
-      <c r="M142" s="43"/>
-      <c r="N142" s="44"/>
-      <c r="O142" s="45"/>
-      <c r="P142" s="43"/>
-      <c r="Q142" s="44"/>
-      <c r="R142" s="44"/>
-      <c r="S142" s="45"/>
+      <c r="C142" s="44"/>
+      <c r="D142" s="45"/>
+      <c r="E142" s="46"/>
+      <c r="F142" s="44"/>
+      <c r="G142" s="45"/>
+      <c r="H142" s="46"/>
+      <c r="I142" s="44"/>
+      <c r="J142" s="45"/>
+      <c r="K142" s="45"/>
+      <c r="L142" s="46"/>
+      <c r="M142" s="44"/>
+      <c r="N142" s="45"/>
+      <c r="O142" s="46"/>
+      <c r="P142" s="44"/>
+      <c r="Q142" s="45"/>
+      <c r="R142" s="45"/>
+      <c r="S142" s="46"/>
       <c r="T142" s="7"/>
       <c r="U142" s="7"/>
       <c r="V142" s="7"/>
@@ -6390,23 +6371,23 @@
     <row r="143" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
-      <c r="C143" s="43"/>
-      <c r="D143" s="44"/>
-      <c r="E143" s="45"/>
-      <c r="F143" s="43"/>
-      <c r="G143" s="44"/>
-      <c r="H143" s="45"/>
-      <c r="I143" s="43"/>
-      <c r="J143" s="44"/>
-      <c r="K143" s="44"/>
-      <c r="L143" s="45"/>
-      <c r="M143" s="43"/>
-      <c r="N143" s="44"/>
-      <c r="O143" s="45"/>
-      <c r="P143" s="43"/>
-      <c r="Q143" s="44"/>
-      <c r="R143" s="44"/>
-      <c r="S143" s="45"/>
+      <c r="C143" s="44"/>
+      <c r="D143" s="45"/>
+      <c r="E143" s="46"/>
+      <c r="F143" s="44"/>
+      <c r="G143" s="45"/>
+      <c r="H143" s="46"/>
+      <c r="I143" s="44"/>
+      <c r="J143" s="45"/>
+      <c r="K143" s="45"/>
+      <c r="L143" s="46"/>
+      <c r="M143" s="44"/>
+      <c r="N143" s="45"/>
+      <c r="O143" s="46"/>
+      <c r="P143" s="44"/>
+      <c r="Q143" s="45"/>
+      <c r="R143" s="45"/>
+      <c r="S143" s="46"/>
       <c r="T143" s="7"/>
       <c r="U143" s="7"/>
       <c r="V143" s="7"/>
@@ -28151,69 +28132,269 @@
     </row>
   </sheetData>
   <mergeCells count="351">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="M120:O120"/>
-    <mergeCell ref="P120:S120"/>
-    <mergeCell ref="I118:L118"/>
-    <mergeCell ref="M118:O118"/>
-    <mergeCell ref="P118:S118"/>
-    <mergeCell ref="I119:L119"/>
-    <mergeCell ref="M119:O119"/>
-    <mergeCell ref="P119:S119"/>
-    <mergeCell ref="I120:L120"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="C63:H63"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="M141:O141"/>
-    <mergeCell ref="P141:S141"/>
-    <mergeCell ref="I142:L142"/>
-    <mergeCell ref="M142:O142"/>
-    <mergeCell ref="P142:S142"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="F139:H139"/>
-    <mergeCell ref="F140:H140"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F141:H141"/>
-    <mergeCell ref="F142:H142"/>
-    <mergeCell ref="M140:O140"/>
-    <mergeCell ref="P140:S140"/>
-    <mergeCell ref="I130:L130"/>
-    <mergeCell ref="I137:L137"/>
-    <mergeCell ref="M137:O137"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:H55"/>
-    <mergeCell ref="P124:S124"/>
-    <mergeCell ref="M127:O127"/>
-    <mergeCell ref="P127:S127"/>
-    <mergeCell ref="I139:L139"/>
-    <mergeCell ref="M139:O139"/>
-    <mergeCell ref="P139:S139"/>
-    <mergeCell ref="I125:L125"/>
-    <mergeCell ref="M125:O125"/>
-    <mergeCell ref="P125:S125"/>
-    <mergeCell ref="M128:O128"/>
-    <mergeCell ref="P128:S128"/>
-    <mergeCell ref="I129:L129"/>
-    <mergeCell ref="M129:O129"/>
-    <mergeCell ref="P129:S129"/>
-    <mergeCell ref="M131:O131"/>
-    <mergeCell ref="P131:S131"/>
-    <mergeCell ref="I132:L132"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="P82:S82"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C82:E82"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="I82:L82"/>
+    <mergeCell ref="M82:O82"/>
+    <mergeCell ref="I87:L87"/>
+    <mergeCell ref="M87:O87"/>
+    <mergeCell ref="P87:S87"/>
+    <mergeCell ref="M88:O88"/>
+    <mergeCell ref="P88:S88"/>
+    <mergeCell ref="I88:L88"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="I89:L89"/>
+    <mergeCell ref="M89:O89"/>
+    <mergeCell ref="P89:S89"/>
+    <mergeCell ref="I90:L90"/>
+    <mergeCell ref="M90:O90"/>
+    <mergeCell ref="P90:S90"/>
+    <mergeCell ref="M93:O93"/>
+    <mergeCell ref="P93:S93"/>
+    <mergeCell ref="I91:L91"/>
+    <mergeCell ref="M91:O91"/>
+    <mergeCell ref="P91:S91"/>
+    <mergeCell ref="I92:L92"/>
+    <mergeCell ref="M92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="I93:L93"/>
+    <mergeCell ref="M96:O96"/>
+    <mergeCell ref="P96:S96"/>
+    <mergeCell ref="I94:L94"/>
+    <mergeCell ref="M94:O94"/>
+    <mergeCell ref="P94:S94"/>
+    <mergeCell ref="I95:L95"/>
+    <mergeCell ref="M95:O95"/>
+    <mergeCell ref="P95:S95"/>
+    <mergeCell ref="I96:L96"/>
+    <mergeCell ref="M99:O99"/>
+    <mergeCell ref="P99:S99"/>
+    <mergeCell ref="I97:L97"/>
+    <mergeCell ref="M97:O97"/>
+    <mergeCell ref="P97:S97"/>
+    <mergeCell ref="I98:L98"/>
+    <mergeCell ref="M98:O98"/>
+    <mergeCell ref="P98:S98"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="M102:O102"/>
+    <mergeCell ref="P102:S102"/>
+    <mergeCell ref="I100:L100"/>
+    <mergeCell ref="M100:O100"/>
+    <mergeCell ref="P100:S100"/>
+    <mergeCell ref="I101:L101"/>
+    <mergeCell ref="M101:O101"/>
+    <mergeCell ref="P101:S101"/>
+    <mergeCell ref="I102:L102"/>
+    <mergeCell ref="M105:O105"/>
+    <mergeCell ref="P105:S105"/>
+    <mergeCell ref="I103:L103"/>
+    <mergeCell ref="M103:O103"/>
+    <mergeCell ref="P103:S103"/>
+    <mergeCell ref="I104:L104"/>
+    <mergeCell ref="M104:O104"/>
+    <mergeCell ref="P104:S104"/>
+    <mergeCell ref="I105:L105"/>
+    <mergeCell ref="M108:O108"/>
+    <mergeCell ref="P108:S108"/>
+    <mergeCell ref="I106:L106"/>
+    <mergeCell ref="M106:O106"/>
+    <mergeCell ref="P106:S106"/>
+    <mergeCell ref="I107:L107"/>
+    <mergeCell ref="M107:O107"/>
+    <mergeCell ref="P107:S107"/>
+    <mergeCell ref="I108:L108"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:H22"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="C96:E96"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="F110:H110"/>
+    <mergeCell ref="F111:H111"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="P122:S122"/>
+    <mergeCell ref="I123:L123"/>
+    <mergeCell ref="I124:L124"/>
+    <mergeCell ref="M124:O124"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="M130:O130"/>
+    <mergeCell ref="P130:S130"/>
+    <mergeCell ref="I128:L128"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="P83:S83"/>
+    <mergeCell ref="I85:L85"/>
+    <mergeCell ref="I86:L86"/>
+    <mergeCell ref="M86:O86"/>
+    <mergeCell ref="P86:S86"/>
+    <mergeCell ref="I83:L83"/>
+    <mergeCell ref="M83:O83"/>
+    <mergeCell ref="I84:L84"/>
+    <mergeCell ref="M84:O84"/>
+    <mergeCell ref="P84:S84"/>
+    <mergeCell ref="M85:O85"/>
+    <mergeCell ref="P85:S85"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="I126:L126"/>
+    <mergeCell ref="M126:O126"/>
+    <mergeCell ref="P126:S126"/>
+    <mergeCell ref="I127:L127"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="M136:O136"/>
+    <mergeCell ref="P136:S136"/>
+    <mergeCell ref="I134:L134"/>
+    <mergeCell ref="M134:O134"/>
+    <mergeCell ref="P134:S134"/>
+    <mergeCell ref="I135:L135"/>
+    <mergeCell ref="M135:O135"/>
+    <mergeCell ref="P135:S135"/>
+    <mergeCell ref="I136:L136"/>
+    <mergeCell ref="M132:O132"/>
+    <mergeCell ref="P132:S132"/>
+    <mergeCell ref="I133:L133"/>
+    <mergeCell ref="M123:O123"/>
+    <mergeCell ref="P123:S123"/>
+    <mergeCell ref="I121:L121"/>
+    <mergeCell ref="M121:O121"/>
+    <mergeCell ref="P121:S121"/>
+    <mergeCell ref="I122:L122"/>
+    <mergeCell ref="I112:L112"/>
+    <mergeCell ref="M112:O112"/>
+    <mergeCell ref="P112:S112"/>
+    <mergeCell ref="I113:L113"/>
+    <mergeCell ref="M113:O113"/>
+    <mergeCell ref="P113:S113"/>
+    <mergeCell ref="I114:L114"/>
+    <mergeCell ref="M114:O114"/>
+    <mergeCell ref="P114:S114"/>
+    <mergeCell ref="M111:O111"/>
+    <mergeCell ref="P111:S111"/>
+    <mergeCell ref="I109:L109"/>
+    <mergeCell ref="M109:O109"/>
+    <mergeCell ref="P109:S109"/>
+    <mergeCell ref="I110:L110"/>
+    <mergeCell ref="M110:O110"/>
+    <mergeCell ref="P110:S110"/>
+    <mergeCell ref="I111:L111"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="C116:E116"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="C141:E141"/>
+    <mergeCell ref="C142:E142"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="C136:E136"/>
+    <mergeCell ref="C137:E137"/>
+    <mergeCell ref="C138:E138"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="C132:E132"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C124:E124"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C126:E126"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="C128:E128"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="M117:O117"/>
+    <mergeCell ref="P117:S117"/>
+    <mergeCell ref="I115:L115"/>
+    <mergeCell ref="M115:O115"/>
+    <mergeCell ref="P115:S115"/>
+    <mergeCell ref="I116:L116"/>
+    <mergeCell ref="M116:O116"/>
+    <mergeCell ref="P116:S116"/>
+    <mergeCell ref="I117:L117"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="F120:H120"/>
     <mergeCell ref="C59:H59"/>
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="I138:L138"/>
@@ -28238,270 +28419,70 @@
     <mergeCell ref="P137:S137"/>
     <mergeCell ref="M133:O133"/>
     <mergeCell ref="P133:S133"/>
+    <mergeCell ref="P124:S124"/>
+    <mergeCell ref="M127:O127"/>
+    <mergeCell ref="P127:S127"/>
+    <mergeCell ref="I139:L139"/>
+    <mergeCell ref="M139:O139"/>
+    <mergeCell ref="P139:S139"/>
+    <mergeCell ref="I125:L125"/>
+    <mergeCell ref="M125:O125"/>
+    <mergeCell ref="P125:S125"/>
+    <mergeCell ref="M128:O128"/>
+    <mergeCell ref="P128:S128"/>
+    <mergeCell ref="I129:L129"/>
+    <mergeCell ref="M129:O129"/>
+    <mergeCell ref="P129:S129"/>
+    <mergeCell ref="M131:O131"/>
+    <mergeCell ref="P131:S131"/>
+    <mergeCell ref="I132:L132"/>
     <mergeCell ref="I131:L131"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="M117:O117"/>
-    <mergeCell ref="P117:S117"/>
-    <mergeCell ref="I115:L115"/>
-    <mergeCell ref="M115:O115"/>
-    <mergeCell ref="P115:S115"/>
-    <mergeCell ref="I116:L116"/>
-    <mergeCell ref="M116:O116"/>
-    <mergeCell ref="P116:S116"/>
-    <mergeCell ref="I117:L117"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="C132:E132"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C124:E124"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="C126:E126"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="C128:E128"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="C130:E130"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="C141:E141"/>
-    <mergeCell ref="C142:E142"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="C133:E133"/>
-    <mergeCell ref="C134:E134"/>
-    <mergeCell ref="C135:E135"/>
-    <mergeCell ref="C136:E136"/>
-    <mergeCell ref="C137:E137"/>
-    <mergeCell ref="C138:E138"/>
-    <mergeCell ref="C139:E139"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="C108:E108"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="C111:E111"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="C116:E116"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="M111:O111"/>
-    <mergeCell ref="P111:S111"/>
-    <mergeCell ref="I109:L109"/>
-    <mergeCell ref="M109:O109"/>
-    <mergeCell ref="P109:S109"/>
-    <mergeCell ref="I110:L110"/>
-    <mergeCell ref="M110:O110"/>
-    <mergeCell ref="P110:S110"/>
-    <mergeCell ref="I111:L111"/>
-    <mergeCell ref="I112:L112"/>
-    <mergeCell ref="M112:O112"/>
-    <mergeCell ref="P112:S112"/>
-    <mergeCell ref="I113:L113"/>
-    <mergeCell ref="M113:O113"/>
-    <mergeCell ref="P113:S113"/>
-    <mergeCell ref="I114:L114"/>
-    <mergeCell ref="M114:O114"/>
-    <mergeCell ref="P114:S114"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="I126:L126"/>
-    <mergeCell ref="M126:O126"/>
-    <mergeCell ref="P126:S126"/>
-    <mergeCell ref="I127:L127"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="M136:O136"/>
-    <mergeCell ref="P136:S136"/>
-    <mergeCell ref="I134:L134"/>
-    <mergeCell ref="M134:O134"/>
-    <mergeCell ref="P134:S134"/>
-    <mergeCell ref="I135:L135"/>
-    <mergeCell ref="M135:O135"/>
-    <mergeCell ref="P135:S135"/>
-    <mergeCell ref="I136:L136"/>
-    <mergeCell ref="M132:O132"/>
-    <mergeCell ref="P132:S132"/>
-    <mergeCell ref="I133:L133"/>
-    <mergeCell ref="M123:O123"/>
-    <mergeCell ref="P123:S123"/>
-    <mergeCell ref="I121:L121"/>
-    <mergeCell ref="M121:O121"/>
-    <mergeCell ref="P121:S121"/>
-    <mergeCell ref="I122:L122"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="P122:S122"/>
-    <mergeCell ref="I123:L123"/>
-    <mergeCell ref="I124:L124"/>
-    <mergeCell ref="M124:O124"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="M130:O130"/>
-    <mergeCell ref="P130:S130"/>
-    <mergeCell ref="I128:L128"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="P83:S83"/>
-    <mergeCell ref="I85:L85"/>
-    <mergeCell ref="I86:L86"/>
-    <mergeCell ref="M86:O86"/>
-    <mergeCell ref="P86:S86"/>
-    <mergeCell ref="I83:L83"/>
-    <mergeCell ref="M83:O83"/>
-    <mergeCell ref="I84:L84"/>
-    <mergeCell ref="M84:O84"/>
-    <mergeCell ref="P84:S84"/>
-    <mergeCell ref="M85:O85"/>
-    <mergeCell ref="P85:S85"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="F110:H110"/>
-    <mergeCell ref="F111:H111"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:H22"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C95:E95"/>
-    <mergeCell ref="C96:E96"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="M108:O108"/>
-    <mergeCell ref="P108:S108"/>
-    <mergeCell ref="I106:L106"/>
-    <mergeCell ref="M106:O106"/>
-    <mergeCell ref="P106:S106"/>
-    <mergeCell ref="I107:L107"/>
-    <mergeCell ref="M107:O107"/>
-    <mergeCell ref="P107:S107"/>
-    <mergeCell ref="I108:L108"/>
-    <mergeCell ref="M105:O105"/>
-    <mergeCell ref="P105:S105"/>
-    <mergeCell ref="I103:L103"/>
-    <mergeCell ref="M103:O103"/>
-    <mergeCell ref="P103:S103"/>
-    <mergeCell ref="I104:L104"/>
-    <mergeCell ref="M104:O104"/>
-    <mergeCell ref="P104:S104"/>
-    <mergeCell ref="I105:L105"/>
-    <mergeCell ref="M102:O102"/>
-    <mergeCell ref="P102:S102"/>
-    <mergeCell ref="I100:L100"/>
-    <mergeCell ref="M100:O100"/>
-    <mergeCell ref="P100:S100"/>
-    <mergeCell ref="I101:L101"/>
-    <mergeCell ref="M101:O101"/>
-    <mergeCell ref="P101:S101"/>
-    <mergeCell ref="I102:L102"/>
-    <mergeCell ref="M99:O99"/>
-    <mergeCell ref="P99:S99"/>
-    <mergeCell ref="I97:L97"/>
-    <mergeCell ref="M97:O97"/>
-    <mergeCell ref="P97:S97"/>
-    <mergeCell ref="I98:L98"/>
-    <mergeCell ref="M98:O98"/>
-    <mergeCell ref="P98:S98"/>
-    <mergeCell ref="I99:L99"/>
-    <mergeCell ref="M96:O96"/>
-    <mergeCell ref="P96:S96"/>
-    <mergeCell ref="I94:L94"/>
-    <mergeCell ref="M94:O94"/>
-    <mergeCell ref="P94:S94"/>
-    <mergeCell ref="I95:L95"/>
-    <mergeCell ref="M95:O95"/>
-    <mergeCell ref="P95:S95"/>
-    <mergeCell ref="I96:L96"/>
-    <mergeCell ref="I89:L89"/>
-    <mergeCell ref="M89:O89"/>
-    <mergeCell ref="P89:S89"/>
-    <mergeCell ref="I90:L90"/>
-    <mergeCell ref="M90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="M93:O93"/>
-    <mergeCell ref="P93:S93"/>
-    <mergeCell ref="I91:L91"/>
-    <mergeCell ref="M91:O91"/>
-    <mergeCell ref="P91:S91"/>
-    <mergeCell ref="I92:L92"/>
-    <mergeCell ref="M92:O92"/>
-    <mergeCell ref="P92:S92"/>
-    <mergeCell ref="I93:L93"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="P82:S82"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:H34"/>
-    <mergeCell ref="C82:E82"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="I82:L82"/>
-    <mergeCell ref="M82:O82"/>
-    <mergeCell ref="I87:L87"/>
-    <mergeCell ref="M87:O87"/>
-    <mergeCell ref="P87:S87"/>
-    <mergeCell ref="M88:O88"/>
-    <mergeCell ref="P88:S88"/>
-    <mergeCell ref="I88:L88"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:H44"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F141:H141"/>
+    <mergeCell ref="F142:H142"/>
+    <mergeCell ref="M140:O140"/>
+    <mergeCell ref="P140:S140"/>
+    <mergeCell ref="I130:L130"/>
+    <mergeCell ref="I137:L137"/>
+    <mergeCell ref="M137:O137"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="M141:O141"/>
+    <mergeCell ref="P141:S141"/>
+    <mergeCell ref="I142:L142"/>
+    <mergeCell ref="M142:O142"/>
+    <mergeCell ref="P142:S142"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="F139:H139"/>
+    <mergeCell ref="F140:H140"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="M120:O120"/>
+    <mergeCell ref="P120:S120"/>
+    <mergeCell ref="I118:L118"/>
+    <mergeCell ref="M118:O118"/>
+    <mergeCell ref="P118:S118"/>
+    <mergeCell ref="I119:L119"/>
+    <mergeCell ref="M119:O119"/>
+    <mergeCell ref="P119:S119"/>
+    <mergeCell ref="I120:L120"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="C63:H63"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:H55"/>
+    <mergeCell ref="A59:B59"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:D2 A3:B4 A1">
     <cfRule type="colorScale" priority="1">
@@ -28519,14 +28500,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c9eb58d-2f4c-499b-ab9c-47c1d5de8bf8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9f673192-3ebd-46cf-81e4-b0fc52a2734b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28719,21 +28698,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c9eb58d-2f4c-499b-ab9c-47c1d5de8bf8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9f673192-3ebd-46cf-81e4-b0fc52a2734b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75874065-9FDF-4780-9B87-C1C24E93EFA3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE45D4B-B629-4110-ABAC-4B0F11E7BBFD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c9eb58d-2f4c-499b-ab9c-47c1d5de8bf8"/>
-    <ds:schemaRef ds:uri="9f673192-3ebd-46cf-81e4-b0fc52a2734b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28758,9 +28736,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE45D4B-B629-4110-ABAC-4B0F11E7BBFD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75874065-9FDF-4780-9B87-C1C24E93EFA3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c9eb58d-2f4c-499b-ab9c-47c1d5de8bf8"/>
+    <ds:schemaRef ds:uri="9f673192-3ebd-46cf-81e4-b0fc52a2734b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>